<commit_message>
Updated on 8 May
</commit_message>
<xml_diff>
--- a/PartnerMasterConfiguration.xlsx
+++ b/PartnerMasterConfiguration.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90450E90-6D9D-4894-B617-D2307D7C6328}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9138FA9F-0030-4606-9C21-FD505D50AC0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Config!$A$1:$AB$190</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mapping!$A$1:$F$1609</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mapping!$A$1:$F$1610</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7724" uniqueCount="1186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7726" uniqueCount="1186">
   <si>
     <t>Partner ID</t>
   </si>
@@ -3679,7 +3679,7 @@
     <t>607417_I</t>
   </si>
   <si>
-    <t>test</t>
+    <t>SBA</t>
   </si>
 </sst>
 </file>
@@ -4706,12 +4706,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AB191"/>
+  <dimension ref="A1:AB190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="A191" sqref="A191"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -16826,7 +16826,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="184" spans="1:21" ht="30.75" thickBot="1">
+    <row r="184" spans="1:21" ht="15.75" thickBot="1">
       <c r="A184" s="7">
         <v>17931</v>
       </c>
@@ -17229,11 +17229,6 @@
       </c>
       <c r="U190" s="16" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="191" spans="1:21">
-      <c r="B191" s="60" t="s">
-        <v>1185</v>
       </c>
     </row>
   </sheetData>
@@ -17413,17 +17408,17 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F1609"/>
+  <dimension ref="A1:F1610"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1551" sqref="A1551:XFD1551"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.85546875" style="39" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="39" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" style="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" style="39" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" style="39" customWidth="1"/>
@@ -17730,7 +17725,7 @@
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1">
+    <row r="25" spans="1:5" ht="30.75" thickBot="1">
       <c r="A25" s="29" t="s">
         <v>694</v>
       </c>
@@ -24767,7 +24762,7 @@
       <c r="D587" s="29"/>
       <c r="E587" s="29"/>
     </row>
-    <row r="588" spans="1:5" ht="15.75" thickBot="1">
+    <row r="588" spans="1:5" ht="30.75" thickBot="1">
       <c r="A588" s="29" t="s">
         <v>684</v>
       </c>
@@ -35308,12 +35303,12 @@
       <c r="E1358" s="32"/>
       <c r="F1358" s="32"/>
     </row>
-    <row r="1359" spans="1:6">
+    <row r="1359" spans="1:6" ht="14.25" customHeight="1">
       <c r="A1359" s="32" t="s">
         <v>1034</v>
       </c>
       <c r="B1359" s="33" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
       <c r="C1359" s="32" t="s">
         <v>1043</v>
@@ -35322,18 +35317,18 @@
       <c r="E1359" s="32"/>
       <c r="F1359" s="32"/>
     </row>
-    <row r="1360" spans="1:6">
+    <row r="1360" spans="1:6" s="41" customFormat="1" ht="14.25" customHeight="1">
       <c r="A1360" s="32" t="s">
-        <v>1044</v>
+        <v>1034</v>
       </c>
       <c r="B1360" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1360" s="32"/>
+        <v>98</v>
+      </c>
+      <c r="C1360" s="32" t="s">
+        <v>1185</v>
+      </c>
       <c r="D1360" s="32"/>
-      <c r="E1360" s="32" t="s">
-        <v>37</v>
-      </c>
+      <c r="E1360" s="32"/>
       <c r="F1360" s="32"/>
     </row>
     <row r="1361" spans="1:6">
@@ -35341,12 +35336,12 @@
         <v>1044</v>
       </c>
       <c r="B1361" s="33" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="C1361" s="32"/>
       <c r="D1361" s="32"/>
       <c r="E1361" s="32" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="F1361" s="32"/>
     </row>
@@ -35355,12 +35350,12 @@
         <v>1044</v>
       </c>
       <c r="B1362" s="33" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C1362" s="32"/>
       <c r="D1362" s="32"/>
       <c r="E1362" s="32" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="F1362" s="32"/>
     </row>
@@ -35368,13 +35363,13 @@
       <c r="A1363" s="32" t="s">
         <v>1044</v>
       </c>
-      <c r="B1363" s="57" t="s">
-        <v>22</v>
+      <c r="B1363" s="33" t="s">
+        <v>95</v>
       </c>
       <c r="C1363" s="32"/>
       <c r="D1363" s="32"/>
       <c r="E1363" s="32" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F1363" s="32"/>
     </row>
@@ -35382,14 +35377,14 @@
       <c r="A1364" s="32" t="s">
         <v>1044</v>
       </c>
-      <c r="B1364" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1364" s="32" t="s">
-        <v>91</v>
-      </c>
+      <c r="B1364" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1364" s="32"/>
       <c r="D1364" s="32"/>
-      <c r="E1364" s="32"/>
+      <c r="E1364" s="32" t="s">
+        <v>23</v>
+      </c>
       <c r="F1364" s="32"/>
     </row>
     <row r="1365" spans="1:6">
@@ -35397,35 +35392,38 @@
         <v>1044</v>
       </c>
       <c r="B1365" s="33" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C1365" s="32" t="s">
-        <v>980</v>
+        <v>91</v>
       </c>
       <c r="D1365" s="32"/>
       <c r="E1365" s="32"/>
       <c r="F1365" s="32"/>
     </row>
     <row r="1366" spans="1:6">
-      <c r="A1366" s="39" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B1366" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1366" s="39" t="s">
-        <v>37</v>
-      </c>
+      <c r="A1366" s="32" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B1366" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1366" s="32" t="s">
+        <v>980</v>
+      </c>
+      <c r="D1366" s="32"/>
+      <c r="E1366" s="32"/>
+      <c r="F1366" s="32"/>
     </row>
     <row r="1367" spans="1:6">
       <c r="A1367" s="39" t="s">
         <v>1095</v>
       </c>
       <c r="B1367" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1367" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1368" spans="1:6">
@@ -35433,10 +35431,10 @@
         <v>1095</v>
       </c>
       <c r="B1368" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1368" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1369" spans="1:6">
@@ -35444,10 +35442,10 @@
         <v>1095</v>
       </c>
       <c r="B1369" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1369" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1370" spans="1:6">
@@ -35455,10 +35453,10 @@
         <v>1095</v>
       </c>
       <c r="B1370" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1370" s="39" t="s">
-        <v>1096</v>
+        <v>22</v>
+      </c>
+      <c r="E1370" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1371" spans="1:6">
@@ -35466,10 +35464,10 @@
         <v>1095</v>
       </c>
       <c r="B1371" s="39" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="C1371" s="39" t="s">
-        <v>172</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="1372" spans="1:6">
@@ -35477,10 +35475,10 @@
         <v>1095</v>
       </c>
       <c r="B1372" s="39" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C1372" s="39" t="s">
-        <v>1047</v>
+        <v>172</v>
       </c>
     </row>
     <row r="1373" spans="1:6">
@@ -35488,10 +35486,10 @@
         <v>1095</v>
       </c>
       <c r="B1373" s="39" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C1373" s="39" t="s">
-        <v>924</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="1374" spans="1:6">
@@ -35499,10 +35497,10 @@
         <v>1095</v>
       </c>
       <c r="B1374" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1374" s="39" t="s">
-        <v>687</v>
+        <v>924</v>
       </c>
     </row>
     <row r="1375" spans="1:6">
@@ -35510,10 +35508,10 @@
         <v>1095</v>
       </c>
       <c r="B1375" s="39" t="s">
-        <v>178</v>
+        <v>78</v>
       </c>
       <c r="C1375" s="39" t="s">
-        <v>179</v>
+        <v>687</v>
       </c>
     </row>
     <row r="1376" spans="1:6">
@@ -35521,10 +35519,10 @@
         <v>1095</v>
       </c>
       <c r="B1376" s="39" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="C1376" s="39" t="s">
-        <v>1097</v>
+        <v>179</v>
       </c>
     </row>
     <row r="1377" spans="1:5">
@@ -35532,10 +35530,10 @@
         <v>1095</v>
       </c>
       <c r="B1377" s="39" t="s">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="C1377" s="39" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="1378" spans="1:5">
@@ -35543,10 +35541,10 @@
         <v>1095</v>
       </c>
       <c r="B1378" s="39" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="C1378" s="39" t="s">
-        <v>1029</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="1379" spans="1:5">
@@ -35554,21 +35552,21 @@
         <v>1095</v>
       </c>
       <c r="B1379" s="39" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C1379" s="39" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="1380" spans="1:5">
       <c r="A1380" s="39" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="B1380" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1380" s="39" t="s">
-        <v>37</v>
+        <v>96</v>
+      </c>
+      <c r="C1380" s="39" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="1381" spans="1:5">
@@ -35576,10 +35574,10 @@
         <v>1099</v>
       </c>
       <c r="B1381" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1381" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1382" spans="1:5">
@@ -35587,10 +35585,10 @@
         <v>1099</v>
       </c>
       <c r="B1382" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1382" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1383" spans="1:5">
@@ -35598,10 +35596,10 @@
         <v>1099</v>
       </c>
       <c r="B1383" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1383" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1384" spans="1:5">
@@ -35609,10 +35607,10 @@
         <v>1099</v>
       </c>
       <c r="B1384" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1384" s="39" t="s">
-        <v>116</v>
+        <v>22</v>
+      </c>
+      <c r="E1384" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1385" spans="1:5">
@@ -35620,21 +35618,21 @@
         <v>1099</v>
       </c>
       <c r="B1385" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1385" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1386" spans="1:5">
       <c r="A1386" s="39" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B1386" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1386" s="39" t="s">
-        <v>37</v>
+        <v>89</v>
+      </c>
+      <c r="C1386" s="39" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="1387" spans="1:5">
@@ -35642,10 +35640,10 @@
         <v>1100</v>
       </c>
       <c r="B1387" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1387" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1388" spans="1:5">
@@ -35653,10 +35651,10 @@
         <v>1100</v>
       </c>
       <c r="B1388" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1388" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1389" spans="1:5">
@@ -35664,10 +35662,10 @@
         <v>1100</v>
       </c>
       <c r="B1389" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1389" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1390" spans="1:5">
@@ -35675,10 +35673,10 @@
         <v>1100</v>
       </c>
       <c r="B1390" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1390" s="39" t="s">
-        <v>349</v>
+        <v>22</v>
+      </c>
+      <c r="E1390" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1391" spans="1:5">
@@ -35686,10 +35684,10 @@
         <v>1100</v>
       </c>
       <c r="B1391" s="39" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="C1391" s="39" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="1392" spans="1:5">
@@ -35697,21 +35695,21 @@
         <v>1100</v>
       </c>
       <c r="B1392" s="39" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C1392" s="39" t="s">
-        <v>307</v>
+        <v>348</v>
       </c>
     </row>
     <row r="1393" spans="1:5">
       <c r="A1393" s="39" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B1393" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1393" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1393" s="39" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="1394" spans="1:5">
@@ -35719,10 +35717,10 @@
         <v>1101</v>
       </c>
       <c r="B1394" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1394" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1395" spans="1:5">
@@ -35730,10 +35728,10 @@
         <v>1101</v>
       </c>
       <c r="B1395" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1395" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1396" spans="1:5">
@@ -35741,10 +35739,10 @@
         <v>1101</v>
       </c>
       <c r="B1396" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1396" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1397" spans="1:5">
@@ -35752,10 +35750,10 @@
         <v>1101</v>
       </c>
       <c r="B1397" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1397" s="39" t="s">
-        <v>347</v>
+        <v>22</v>
+      </c>
+      <c r="E1397" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1398" spans="1:5">
@@ -35763,10 +35761,10 @@
         <v>1101</v>
       </c>
       <c r="B1398" s="39" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C1398" s="39" t="s">
-        <v>307</v>
+        <v>347</v>
       </c>
     </row>
     <row r="1399" spans="1:5">
@@ -35774,21 +35772,21 @@
         <v>1101</v>
       </c>
       <c r="B1399" s="39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C1399" s="39" t="s">
-        <v>348</v>
+        <v>307</v>
       </c>
     </row>
     <row r="1400" spans="1:5">
       <c r="A1400" s="39" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B1400" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1400" s="39" t="s">
-        <v>37</v>
+        <v>106</v>
+      </c>
+      <c r="C1400" s="39" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="1401" spans="1:5">
@@ -35796,10 +35794,10 @@
         <v>1102</v>
       </c>
       <c r="B1401" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1401" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1402" spans="1:5">
@@ -35807,10 +35805,10 @@
         <v>1102</v>
       </c>
       <c r="B1402" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1402" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1403" spans="1:5">
@@ -35818,10 +35816,10 @@
         <v>1102</v>
       </c>
       <c r="B1403" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1403" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1404" spans="1:5">
@@ -35829,10 +35827,10 @@
         <v>1102</v>
       </c>
       <c r="B1404" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1404" s="39" t="s">
-        <v>385</v>
+        <v>22</v>
+      </c>
+      <c r="E1404" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1405" spans="1:5">
@@ -35840,10 +35838,10 @@
         <v>1102</v>
       </c>
       <c r="B1405" s="39" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="C1405" s="39" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="1406" spans="1:5">
@@ -35851,21 +35849,21 @@
         <v>1102</v>
       </c>
       <c r="B1406" s="39" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C1406" s="39" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="1407" spans="1:5">
       <c r="A1407" s="39" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B1407" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1407" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1407" s="39" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="1408" spans="1:5">
@@ -35873,10 +35871,10 @@
         <v>1103</v>
       </c>
       <c r="B1408" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1408" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1409" spans="1:5">
@@ -35884,10 +35882,10 @@
         <v>1103</v>
       </c>
       <c r="B1409" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1409" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1410" spans="1:5">
@@ -35895,10 +35893,10 @@
         <v>1103</v>
       </c>
       <c r="B1410" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1410" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1411" spans="1:5">
@@ -35906,10 +35904,10 @@
         <v>1103</v>
       </c>
       <c r="B1411" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1411" s="39" t="s">
-        <v>385</v>
+        <v>22</v>
+      </c>
+      <c r="E1411" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1412" spans="1:5">
@@ -35917,10 +35915,10 @@
         <v>1103</v>
       </c>
       <c r="B1412" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1412" s="39" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="1413" spans="1:5">
@@ -35928,21 +35926,21 @@
         <v>1103</v>
       </c>
       <c r="B1413" s="39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C1413" s="39" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="1414" spans="1:5">
       <c r="A1414" s="39" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B1414" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1414" s="39" t="s">
-        <v>37</v>
+        <v>106</v>
+      </c>
+      <c r="C1414" s="39" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1415" spans="1:5">
@@ -35950,10 +35948,10 @@
         <v>1104</v>
       </c>
       <c r="B1415" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1415" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1416" spans="1:5">
@@ -35961,10 +35959,10 @@
         <v>1104</v>
       </c>
       <c r="B1416" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1416" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1417" spans="1:5">
@@ -35972,10 +35970,10 @@
         <v>1104</v>
       </c>
       <c r="B1417" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1417" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1418" spans="1:5">
@@ -35983,10 +35981,10 @@
         <v>1104</v>
       </c>
       <c r="B1418" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1418" s="39" t="s">
-        <v>356</v>
+        <v>22</v>
+      </c>
+      <c r="E1418" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1419" spans="1:5">
@@ -35994,10 +35992,10 @@
         <v>1104</v>
       </c>
       <c r="B1419" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1419" s="39" t="s">
-        <v>1106</v>
+        <v>356</v>
       </c>
     </row>
     <row r="1420" spans="1:5">
@@ -36005,21 +36003,21 @@
         <v>1104</v>
       </c>
       <c r="B1420" s="39" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C1420" s="39" t="s">
-        <v>1057</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="1421" spans="1:5">
       <c r="A1421" s="39" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="B1421" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1421" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1421" s="39" t="s">
+        <v>1057</v>
       </c>
     </row>
     <row r="1422" spans="1:5">
@@ -36027,10 +36025,10 @@
         <v>1107</v>
       </c>
       <c r="B1422" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1422" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1423" spans="1:5">
@@ -36038,10 +36036,10 @@
         <v>1107</v>
       </c>
       <c r="B1423" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1423" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1424" spans="1:5">
@@ -36049,10 +36047,10 @@
         <v>1107</v>
       </c>
       <c r="B1424" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1424" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1425" spans="1:5">
@@ -36060,10 +36058,10 @@
         <v>1107</v>
       </c>
       <c r="B1425" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1425" s="39" t="s">
-        <v>356</v>
+        <v>22</v>
+      </c>
+      <c r="E1425" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1426" spans="1:5">
@@ -36071,10 +36069,10 @@
         <v>1107</v>
       </c>
       <c r="B1426" s="39" t="s">
-        <v>97</v>
+        <v>27</v>
       </c>
       <c r="C1426" s="39" t="s">
-        <v>1105</v>
+        <v>356</v>
       </c>
     </row>
     <row r="1427" spans="1:5">
@@ -36082,10 +36080,10 @@
         <v>1107</v>
       </c>
       <c r="B1427" s="39" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C1427" s="39" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="1428" spans="1:5">
@@ -36093,21 +36091,21 @@
         <v>1107</v>
       </c>
       <c r="B1428" s="39" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C1428" s="39" t="s">
-        <v>1058</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="1429" spans="1:5">
       <c r="A1429" s="39" t="s">
-        <v>1148</v>
+        <v>1107</v>
       </c>
       <c r="B1429" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1429" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1429" s="39" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="1430" spans="1:5">
@@ -36115,10 +36113,10 @@
         <v>1148</v>
       </c>
       <c r="B1430" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1430" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1431" spans="1:5">
@@ -36126,10 +36124,10 @@
         <v>1148</v>
       </c>
       <c r="B1431" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1431" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1432" spans="1:5">
@@ -36137,10 +36135,10 @@
         <v>1148</v>
       </c>
       <c r="B1432" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1432" s="39" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="E1432" s="39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="1433" spans="1:5">
@@ -36148,10 +36146,10 @@
         <v>1148</v>
       </c>
       <c r="B1433" s="39" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1433" s="39" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1434" spans="1:5">
@@ -36159,10 +36157,10 @@
         <v>1148</v>
       </c>
       <c r="B1434" s="39" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="C1434" s="39" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
     </row>
     <row r="1435" spans="1:5">
@@ -36170,10 +36168,10 @@
         <v>1148</v>
       </c>
       <c r="B1435" s="39" t="s">
-        <v>206</v>
+        <v>94</v>
       </c>
       <c r="C1435" s="39" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="1436" spans="1:5">
@@ -36181,10 +36179,10 @@
         <v>1148</v>
       </c>
       <c r="B1436" s="39" t="s">
-        <v>985</v>
+        <v>206</v>
       </c>
       <c r="C1436" s="39" t="s">
-        <v>1024</v>
+        <v>101</v>
       </c>
     </row>
     <row r="1437" spans="1:5">
@@ -36192,10 +36190,10 @@
         <v>1148</v>
       </c>
       <c r="B1437" s="39" t="s">
-        <v>178</v>
+        <v>985</v>
       </c>
       <c r="C1437" s="39" t="s">
-        <v>103</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="1438" spans="1:5">
@@ -36203,10 +36201,10 @@
         <v>1148</v>
       </c>
       <c r="B1438" s="39" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="C1438" s="39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="1439" spans="1:5">
@@ -36214,10 +36212,10 @@
         <v>1148</v>
       </c>
       <c r="B1439" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1439" s="39" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="1440" spans="1:5">
@@ -36225,21 +36223,21 @@
         <v>1148</v>
       </c>
       <c r="B1440" s="39" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
       <c r="C1440" s="39" t="s">
-        <v>1028</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1441" spans="1:5">
       <c r="A1441" s="39" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B1441" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1441" s="39" t="s">
-        <v>37</v>
+        <v>160</v>
+      </c>
+      <c r="C1441" s="39" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="1442" spans="1:5">
@@ -36247,10 +36245,10 @@
         <v>1149</v>
       </c>
       <c r="B1442" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1442" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1443" spans="1:5">
@@ -36258,10 +36256,10 @@
         <v>1149</v>
       </c>
       <c r="B1443" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1443" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1444" spans="1:5">
@@ -36269,10 +36267,10 @@
         <v>1149</v>
       </c>
       <c r="B1444" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1444" s="39" t="s">
-        <v>100</v>
+        <v>95</v>
+      </c>
+      <c r="E1444" s="39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="1445" spans="1:5">
@@ -36280,10 +36278,10 @@
         <v>1149</v>
       </c>
       <c r="B1445" s="39" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1445" s="39" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1446" spans="1:5">
@@ -36291,10 +36289,10 @@
         <v>1149</v>
       </c>
       <c r="B1446" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1446" s="39" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="1447" spans="1:5">
@@ -36302,21 +36300,21 @@
         <v>1149</v>
       </c>
       <c r="B1447" s="39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C1447" s="39" t="s">
-        <v>342</v>
+        <v>70</v>
       </c>
     </row>
     <row r="1448" spans="1:5">
       <c r="A1448" s="39" t="s">
-        <v>981</v>
+        <v>1149</v>
       </c>
       <c r="B1448" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1448" s="39" t="s">
-        <v>37</v>
+        <v>106</v>
+      </c>
+      <c r="C1448" s="39" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="1449" spans="1:5">
@@ -36324,32 +36322,32 @@
         <v>981</v>
       </c>
       <c r="B1449" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1449" s="39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="1450" spans="1:5" ht="14.25" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:5">
       <c r="A1450" s="39" t="s">
         <v>981</v>
       </c>
       <c r="B1450" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1450" s="39" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="1451" spans="1:5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1451" s="39" t="s">
         <v>981</v>
       </c>
       <c r="B1451" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1451" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1452" spans="1:5">
@@ -36357,10 +36355,10 @@
         <v>981</v>
       </c>
       <c r="B1452" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1452" s="39" t="s">
-        <v>939</v>
+        <v>22</v>
+      </c>
+      <c r="E1452" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1453" spans="1:5">
@@ -36368,10 +36366,10 @@
         <v>981</v>
       </c>
       <c r="B1453" s="39" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="C1453" s="39" t="s">
-        <v>172</v>
+        <v>939</v>
       </c>
     </row>
     <row r="1454" spans="1:5">
@@ -36379,21 +36377,21 @@
         <v>981</v>
       </c>
       <c r="B1454" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1454" s="39">
-        <v>8</v>
+        <v>106</v>
+      </c>
+      <c r="C1454" s="39" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="1455" spans="1:5">
       <c r="A1455" s="39" t="s">
-        <v>1147</v>
+        <v>981</v>
       </c>
       <c r="B1455" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1455" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1455" s="39">
+        <v>8</v>
       </c>
     </row>
     <row r="1456" spans="1:5">
@@ -36401,10 +36399,10 @@
         <v>1147</v>
       </c>
       <c r="B1456" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1456" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1457" spans="1:5">
@@ -36412,10 +36410,10 @@
         <v>1147</v>
       </c>
       <c r="B1457" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1457" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1458" spans="1:5">
@@ -36423,10 +36421,10 @@
         <v>1147</v>
       </c>
       <c r="B1458" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1458" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1459" spans="1:5">
@@ -36434,10 +36432,10 @@
         <v>1147</v>
       </c>
       <c r="B1459" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1459" s="39" t="s">
-        <v>1108</v>
+        <v>22</v>
+      </c>
+      <c r="E1459" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1460" spans="1:5">
@@ -36445,10 +36443,10 @@
         <v>1147</v>
       </c>
       <c r="B1460" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1460" s="39" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1461" spans="1:5">
@@ -36456,21 +36454,21 @@
         <v>1147</v>
       </c>
       <c r="B1461" s="39" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C1461" s="39" t="s">
-        <v>1067</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1462" spans="1:5">
       <c r="A1462" s="39" t="s">
-        <v>1110</v>
+        <v>1147</v>
       </c>
       <c r="B1462" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1462" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1462" s="39" t="s">
+        <v>1067</v>
       </c>
     </row>
     <row r="1463" spans="1:5">
@@ -36478,10 +36476,10 @@
         <v>1110</v>
       </c>
       <c r="B1463" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1463" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1464" spans="1:5">
@@ -36489,10 +36487,10 @@
         <v>1110</v>
       </c>
       <c r="B1464" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1464" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1465" spans="1:5">
@@ -36500,10 +36498,10 @@
         <v>1110</v>
       </c>
       <c r="B1465" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1465" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1466" spans="1:5">
@@ -36511,10 +36509,10 @@
         <v>1110</v>
       </c>
       <c r="B1466" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1466" s="39" t="s">
-        <v>1111</v>
+        <v>22</v>
+      </c>
+      <c r="E1466" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1467" spans="1:5">
@@ -36522,10 +36520,10 @@
         <v>1110</v>
       </c>
       <c r="B1467" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1467" s="39" t="s">
-        <v>1072</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="1468" spans="1:5">
@@ -36533,10 +36531,10 @@
         <v>1110</v>
       </c>
       <c r="B1468" s="39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C1468" s="39" t="s">
-        <v>1112</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="1469" spans="1:5">
@@ -36544,21 +36542,21 @@
         <v>1110</v>
       </c>
       <c r="B1469" s="39" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C1469" s="39" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="1470" spans="1:5">
       <c r="A1470" s="39" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="B1470" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1470" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1470" s="39" t="s">
+        <v>1113</v>
       </c>
     </row>
     <row r="1471" spans="1:5">
@@ -36566,10 +36564,10 @@
         <v>1114</v>
       </c>
       <c r="B1471" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1471" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1472" spans="1:5">
@@ -36577,10 +36575,10 @@
         <v>1114</v>
       </c>
       <c r="B1472" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1472" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1473" spans="1:5">
@@ -36588,10 +36586,10 @@
         <v>1114</v>
       </c>
       <c r="B1473" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1473" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1474" spans="1:5">
@@ -36599,10 +36597,10 @@
         <v>1114</v>
       </c>
       <c r="B1474" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1474" s="39" t="s">
-        <v>1008</v>
+        <v>22</v>
+      </c>
+      <c r="E1474" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1475" spans="1:5">
@@ -36610,21 +36608,21 @@
         <v>1114</v>
       </c>
       <c r="B1475" s="39" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C1475" s="39" t="s">
-        <v>958</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="1476" spans="1:5">
       <c r="A1476" s="39" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B1476" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1476" s="39" t="s">
-        <v>37</v>
+        <v>89</v>
+      </c>
+      <c r="C1476" s="39" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="1477" spans="1:5">
@@ -36632,10 +36630,10 @@
         <v>1115</v>
       </c>
       <c r="B1477" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1477" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1478" spans="1:5">
@@ -36643,10 +36641,10 @@
         <v>1115</v>
       </c>
       <c r="B1478" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1478" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1479" spans="1:5">
@@ -36654,10 +36652,10 @@
         <v>1115</v>
       </c>
       <c r="B1479" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1479" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1480" spans="1:5">
@@ -36665,10 +36663,10 @@
         <v>1115</v>
       </c>
       <c r="B1480" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1480" s="39" t="s">
-        <v>1116</v>
+        <v>22</v>
+      </c>
+      <c r="E1480" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1481" spans="1:5">
@@ -36676,10 +36674,10 @@
         <v>1115</v>
       </c>
       <c r="B1481" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1481" s="39" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="1482" spans="1:5">
@@ -36687,21 +36685,21 @@
         <v>1115</v>
       </c>
       <c r="B1482" s="39" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C1482" s="39" t="s">
-        <v>1080</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="1483" spans="1:5">
       <c r="A1483" s="39" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="B1483" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1483" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1483" s="39" t="s">
+        <v>1080</v>
       </c>
     </row>
     <row r="1484" spans="1:5">
@@ -36709,10 +36707,10 @@
         <v>1118</v>
       </c>
       <c r="B1484" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1484" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1485" spans="1:5">
@@ -36720,10 +36718,10 @@
         <v>1118</v>
       </c>
       <c r="B1485" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1485" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1486" spans="1:5">
@@ -36731,10 +36729,10 @@
         <v>1118</v>
       </c>
       <c r="B1486" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1486" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1487" spans="1:5">
@@ -36742,10 +36740,10 @@
         <v>1118</v>
       </c>
       <c r="B1487" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1487" s="39" t="s">
-        <v>99</v>
+        <v>22</v>
+      </c>
+      <c r="E1487" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1488" spans="1:5">
@@ -36753,10 +36751,10 @@
         <v>1118</v>
       </c>
       <c r="B1488" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1488" s="39">
-        <v>8</v>
+        <v>27</v>
+      </c>
+      <c r="C1488" s="39" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="1489" spans="1:5">
@@ -36764,10 +36762,10 @@
         <v>1118</v>
       </c>
       <c r="B1489" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1489" s="39" t="s">
-        <v>1119</v>
+        <v>89</v>
+      </c>
+      <c r="C1489" s="39">
+        <v>8</v>
       </c>
     </row>
     <row r="1490" spans="1:5">
@@ -36775,21 +36773,21 @@
         <v>1118</v>
       </c>
       <c r="B1490" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1490" s="39">
-        <v>9</v>
+        <v>106</v>
+      </c>
+      <c r="C1490" s="39" t="s">
+        <v>1119</v>
       </c>
     </row>
     <row r="1491" spans="1:5">
       <c r="A1491" s="39" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="B1491" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1491" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1491" s="39">
+        <v>9</v>
       </c>
     </row>
     <row r="1492" spans="1:5">
@@ -36797,10 +36795,10 @@
         <v>1120</v>
       </c>
       <c r="B1492" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1492" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1493" spans="1:5">
@@ -36808,10 +36806,10 @@
         <v>1120</v>
       </c>
       <c r="B1493" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1493" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1494" spans="1:5">
@@ -36819,10 +36817,10 @@
         <v>1120</v>
       </c>
       <c r="B1494" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1494" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1495" spans="1:5">
@@ -36830,10 +36828,10 @@
         <v>1120</v>
       </c>
       <c r="B1495" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1495" s="39" t="s">
-        <v>223</v>
+        <v>22</v>
+      </c>
+      <c r="E1495" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1496" spans="1:5">
@@ -36841,10 +36839,10 @@
         <v>1120</v>
       </c>
       <c r="B1496" s="39" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="C1496" s="39" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
     </row>
     <row r="1497" spans="1:5">
@@ -36852,10 +36850,10 @@
         <v>1120</v>
       </c>
       <c r="B1497" s="39" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C1497" s="39" t="s">
-        <v>1121</v>
+        <v>198</v>
       </c>
     </row>
     <row r="1498" spans="1:5">
@@ -36863,10 +36861,10 @@
         <v>1120</v>
       </c>
       <c r="B1498" s="39" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C1498" s="39" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1499" spans="1:5">
@@ -36874,10 +36872,10 @@
         <v>1120</v>
       </c>
       <c r="B1499" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1499" s="39" t="s">
-        <v>207</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1500" spans="1:5">
@@ -36885,10 +36883,10 @@
         <v>1120</v>
       </c>
       <c r="B1500" s="39" t="s">
-        <v>178</v>
+        <v>78</v>
       </c>
       <c r="C1500" s="39" t="s">
-        <v>1123</v>
+        <v>207</v>
       </c>
     </row>
     <row r="1501" spans="1:5">
@@ -36896,21 +36894,21 @@
         <v>1120</v>
       </c>
       <c r="B1501" s="39" t="s">
-        <v>97</v>
+        <v>178</v>
       </c>
       <c r="C1501" s="39" t="s">
-        <v>210</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1502" spans="1:5">
       <c r="A1502" s="39" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="B1502" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1502" s="39" t="s">
-        <v>37</v>
+        <v>97</v>
+      </c>
+      <c r="C1502" s="39" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="1503" spans="1:5">
@@ -36918,10 +36916,10 @@
         <v>1124</v>
       </c>
       <c r="B1503" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1503" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1504" spans="1:5">
@@ -36929,10 +36927,10 @@
         <v>1124</v>
       </c>
       <c r="B1504" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1504" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1505" spans="1:5">
@@ -36940,10 +36938,10 @@
         <v>1124</v>
       </c>
       <c r="B1505" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1505" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1506" spans="1:5">
@@ -36951,10 +36949,10 @@
         <v>1124</v>
       </c>
       <c r="B1506" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1506" s="39" t="s">
-        <v>1088</v>
+        <v>22</v>
+      </c>
+      <c r="E1506" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1507" spans="1:5">
@@ -36962,21 +36960,21 @@
         <v>1124</v>
       </c>
       <c r="B1507" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1507" s="39" t="s">
-        <v>260</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="1508" spans="1:5">
       <c r="A1508" s="39" t="s">
-        <v>1145</v>
+        <v>1124</v>
       </c>
       <c r="B1508" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1508" s="39" t="s">
-        <v>37</v>
+        <v>89</v>
+      </c>
+      <c r="C1508" s="39" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="1509" spans="1:5">
@@ -36984,10 +36982,10 @@
         <v>1145</v>
       </c>
       <c r="B1509" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1509" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1510" spans="1:5">
@@ -36995,10 +36993,10 @@
         <v>1145</v>
       </c>
       <c r="B1510" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1510" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1511" spans="1:5">
@@ -37006,10 +37004,10 @@
         <v>1145</v>
       </c>
       <c r="B1511" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1511" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1512" spans="1:5">
@@ -37017,10 +37015,10 @@
         <v>1145</v>
       </c>
       <c r="B1512" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1512" s="39" t="s">
-        <v>870</v>
+        <v>22</v>
+      </c>
+      <c r="E1512" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1513" spans="1:5">
@@ -37028,10 +37026,10 @@
         <v>1145</v>
       </c>
       <c r="B1513" s="39" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="C1513" s="39" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="1514" spans="1:5">
@@ -37039,10 +37037,10 @@
         <v>1145</v>
       </c>
       <c r="B1514" s="39" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C1514" s="39" t="s">
-        <v>833</v>
+        <v>871</v>
       </c>
     </row>
     <row r="1515" spans="1:5">
@@ -37050,10 +37048,10 @@
         <v>1145</v>
       </c>
       <c r="B1515" s="39" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C1515" s="39" t="s">
-        <v>873</v>
+        <v>833</v>
       </c>
     </row>
     <row r="1516" spans="1:5">
@@ -37061,21 +37059,21 @@
         <v>1145</v>
       </c>
       <c r="B1516" s="39" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C1516" s="39" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="1517" spans="1:5">
       <c r="A1517" s="39" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B1517" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1517" s="39" t="s">
-        <v>37</v>
+        <v>97</v>
+      </c>
+      <c r="C1517" s="39" t="s">
+        <v>874</v>
       </c>
     </row>
     <row r="1518" spans="1:5">
@@ -37083,10 +37081,10 @@
         <v>1146</v>
       </c>
       <c r="B1518" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1518" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1519" spans="1:5">
@@ -37094,10 +37092,10 @@
         <v>1146</v>
       </c>
       <c r="B1519" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1519" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1520" spans="1:5">
@@ -37105,10 +37103,10 @@
         <v>1146</v>
       </c>
       <c r="B1520" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1520" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1521" spans="1:5">
@@ -37116,10 +37114,10 @@
         <v>1146</v>
       </c>
       <c r="B1521" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1521" s="39" t="s">
-        <v>870</v>
+        <v>22</v>
+      </c>
+      <c r="E1521" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1522" spans="1:5">
@@ -37127,10 +37125,10 @@
         <v>1146</v>
       </c>
       <c r="B1522" s="39" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C1522" s="39" t="s">
-        <v>1091</v>
+        <v>870</v>
       </c>
     </row>
     <row r="1523" spans="1:5">
@@ -37138,10 +37136,10 @@
         <v>1146</v>
       </c>
       <c r="B1523" s="39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C1523" s="39" t="s">
-        <v>871</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="1524" spans="1:5">
@@ -37149,21 +37147,21 @@
         <v>1146</v>
       </c>
       <c r="B1524" s="39" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C1524" s="39" t="s">
-        <v>387</v>
+        <v>871</v>
       </c>
     </row>
     <row r="1525" spans="1:5">
       <c r="A1525" s="39" t="s">
-        <v>1125</v>
+        <v>1146</v>
       </c>
       <c r="B1525" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1525" s="39" t="s">
-        <v>37</v>
+        <v>97</v>
+      </c>
+      <c r="C1525" s="39" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="1526" spans="1:5">
@@ -37171,10 +37169,10 @@
         <v>1125</v>
       </c>
       <c r="B1526" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1526" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1527" spans="1:5">
@@ -37182,10 +37180,10 @@
         <v>1125</v>
       </c>
       <c r="B1527" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1527" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1528" spans="1:5">
@@ -37193,10 +37191,10 @@
         <v>1125</v>
       </c>
       <c r="B1528" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1528" s="39" t="s">
-        <v>1126</v>
+        <v>95</v>
+      </c>
+      <c r="E1528" s="39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="1529" spans="1:5">
@@ -37204,10 +37202,10 @@
         <v>1125</v>
       </c>
       <c r="B1529" s="39" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1529" s="39" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1530" spans="1:5">
@@ -37215,10 +37213,10 @@
         <v>1125</v>
       </c>
       <c r="B1530" s="39" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="C1530" s="39" t="s">
-        <v>1094</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1531" spans="1:5">
@@ -37226,10 +37224,10 @@
         <v>1125</v>
       </c>
       <c r="B1531" s="39" t="s">
-        <v>424</v>
+        <v>94</v>
       </c>
       <c r="C1531" s="39" t="s">
-        <v>1128</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="1532" spans="1:5">
@@ -37237,10 +37235,10 @@
         <v>1125</v>
       </c>
       <c r="B1532" s="39" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C1532" s="39" t="s">
-        <v>451</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1533" spans="1:5">
@@ -37248,10 +37246,10 @@
         <v>1125</v>
       </c>
       <c r="B1533" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C1533" s="39" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="1534" spans="1:5">
@@ -37259,10 +37257,10 @@
         <v>1125</v>
       </c>
       <c r="B1534" s="39" t="s">
-        <v>1129</v>
+        <v>426</v>
       </c>
       <c r="C1534" s="39" t="s">
-        <v>1130</v>
+        <v>452</v>
       </c>
     </row>
     <row r="1535" spans="1:5">
@@ -37270,10 +37268,10 @@
         <v>1125</v>
       </c>
       <c r="B1535" s="39" t="s">
-        <v>427</v>
+        <v>1129</v>
       </c>
       <c r="C1535" s="39" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1536" spans="1:5">
@@ -37281,10 +37279,10 @@
         <v>1125</v>
       </c>
       <c r="B1536" s="39" t="s">
-        <v>1132</v>
+        <v>427</v>
       </c>
       <c r="C1536" s="39" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1537" spans="1:5">
@@ -37292,10 +37290,10 @@
         <v>1125</v>
       </c>
       <c r="B1537" s="39" t="s">
-        <v>168</v>
+        <v>1132</v>
       </c>
       <c r="C1537" s="39" t="s">
-        <v>474</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="1538" spans="1:5">
@@ -37303,10 +37301,10 @@
         <v>1125</v>
       </c>
       <c r="B1538" s="39" t="s">
-        <v>428</v>
+        <v>168</v>
       </c>
       <c r="C1538" s="39" t="s">
-        <v>1134</v>
+        <v>474</v>
       </c>
     </row>
     <row r="1539" spans="1:5">
@@ -37314,10 +37312,10 @@
         <v>1125</v>
       </c>
       <c r="B1539" s="39" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C1539" s="39" t="s">
-        <v>476</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1540" spans="1:5">
@@ -37325,10 +37323,10 @@
         <v>1125</v>
       </c>
       <c r="B1540" s="39" t="s">
-        <v>1135</v>
+        <v>429</v>
       </c>
       <c r="C1540" s="39" t="s">
-        <v>1136</v>
+        <v>476</v>
       </c>
     </row>
     <row r="1541" spans="1:5">
@@ -37336,10 +37334,10 @@
         <v>1125</v>
       </c>
       <c r="B1541" s="39" t="s">
-        <v>430</v>
+        <v>1135</v>
       </c>
       <c r="C1541" s="39" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="1542" spans="1:5">
@@ -37347,10 +37345,10 @@
         <v>1125</v>
       </c>
       <c r="B1542" s="39" t="s">
-        <v>160</v>
+        <v>430</v>
       </c>
       <c r="C1542" s="39" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="1543" spans="1:5">
@@ -37358,10 +37356,10 @@
         <v>1125</v>
       </c>
       <c r="B1543" s="39" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="C1543" s="39" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="1544" spans="1:5">
@@ -37369,37 +37367,37 @@
         <v>1125</v>
       </c>
       <c r="B1544" s="39" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C1544" s="39" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="1545" spans="1:5">
       <c r="A1545" s="39" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B1545" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1545" s="39" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:5">
+      <c r="A1546" s="39" t="s">
         <v>1104</v>
-      </c>
-      <c r="B1545" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1545" s="39" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="1546" spans="1:5" s="6" customFormat="1">
-      <c r="A1546" s="6" t="s">
-        <v>1102</v>
       </c>
       <c r="B1546" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="C1546" s="6" t="s">
-        <v>387</v>
+      <c r="C1546" s="39" t="s">
+        <v>1105</v>
       </c>
     </row>
     <row r="1547" spans="1:5" s="6" customFormat="1">
       <c r="A1547" s="6" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B1547" s="39" t="s">
         <v>97</v>
@@ -37408,15 +37406,15 @@
         <v>387</v>
       </c>
     </row>
-    <row r="1548" spans="1:5">
-      <c r="A1548" s="39" t="s">
-        <v>1153</v>
+    <row r="1548" spans="1:5" s="6" customFormat="1">
+      <c r="A1548" s="6" t="s">
+        <v>1103</v>
       </c>
       <c r="B1548" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1548" s="39" t="s">
-        <v>37</v>
+        <v>97</v>
+      </c>
+      <c r="C1548" s="6" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="1549" spans="1:5">
@@ -37424,10 +37422,10 @@
         <v>1153</v>
       </c>
       <c r="B1549" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1549" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1550" spans="1:5">
@@ -37435,10 +37433,10 @@
         <v>1153</v>
       </c>
       <c r="B1550" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1550" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1551" spans="1:5">
@@ -37446,10 +37444,10 @@
         <v>1153</v>
       </c>
       <c r="B1551" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1551" s="39" t="s">
-        <v>1126</v>
+        <v>95</v>
+      </c>
+      <c r="E1551" s="39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="1552" spans="1:5">
@@ -37457,186 +37455,186 @@
         <v>1153</v>
       </c>
       <c r="B1552" s="39" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1552" s="39" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1553" spans="1:5">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:3">
       <c r="A1553" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1553" s="39" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="C1553" s="39" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="1554" spans="1:5">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:3">
       <c r="A1554" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1554" s="39" t="s">
-        <v>424</v>
+        <v>94</v>
       </c>
       <c r="C1554" s="39" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="1555" spans="1:5">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:3">
       <c r="A1555" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1555" s="39" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C1555" s="39" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="1556" spans="1:5">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:3">
       <c r="A1556" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1556" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C1556" s="39" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="1557" spans="1:5">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:3">
       <c r="A1557" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1557" s="39" t="s">
-        <v>1129</v>
+        <v>426</v>
       </c>
       <c r="C1557" s="39" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="1558" spans="1:5">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:3">
       <c r="A1558" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1558" s="39" t="s">
-        <v>427</v>
+        <v>1129</v>
       </c>
       <c r="C1558" s="39" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="1559" spans="1:5">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:3">
       <c r="A1559" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1559" s="39" t="s">
-        <v>1132</v>
+        <v>427</v>
       </c>
       <c r="C1559" s="39" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="1560" spans="1:5">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:3">
       <c r="A1560" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1560" s="39" t="s">
-        <v>168</v>
+        <v>1132</v>
       </c>
       <c r="C1560" s="39" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="1561" spans="1:5">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:3">
       <c r="A1561" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1561" s="39" t="s">
-        <v>428</v>
+        <v>168</v>
       </c>
       <c r="C1561" s="39" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="1562" spans="1:5">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:3">
       <c r="A1562" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1562" s="39" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C1562" s="39" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="1563" spans="1:5">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:3">
       <c r="A1563" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1563" s="39" t="s">
-        <v>1135</v>
+        <v>429</v>
       </c>
       <c r="C1563" s="39" t="s">
-        <v>1136</v>
-      </c>
-    </row>
-    <row r="1564" spans="1:5">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:3">
       <c r="A1564" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1564" s="39" t="s">
-        <v>430</v>
+        <v>1135</v>
       </c>
       <c r="C1564" s="39" t="s">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="1565" spans="1:5">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:3">
       <c r="A1565" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1565" s="39" t="s">
-        <v>160</v>
+        <v>430</v>
       </c>
       <c r="C1565" s="39" t="s">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="1566" spans="1:5">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:3">
       <c r="A1566" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1566" s="39" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="C1566" s="39" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="1567" spans="1:5">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:3">
       <c r="A1567" s="39" t="s">
         <v>1153</v>
       </c>
       <c r="B1567" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1567" s="39" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:3">
+      <c r="A1568" s="39" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B1568" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C1567" s="39" t="s">
+      <c r="C1568" s="39" t="s">
         <v>1140</v>
-      </c>
-    </row>
-    <row r="1568" spans="1:5">
-      <c r="A1568" s="39" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B1568" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1568" s="39" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="1569" spans="1:5">
@@ -37644,10 +37642,10 @@
         <v>1161</v>
       </c>
       <c r="B1569" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1569" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1570" spans="1:5">
@@ -37655,10 +37653,10 @@
         <v>1161</v>
       </c>
       <c r="B1570" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1570" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1571" spans="1:5">
@@ -37666,10 +37664,10 @@
         <v>1161</v>
       </c>
       <c r="B1571" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1571" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1572" spans="1:5">
@@ -37677,10 +37675,10 @@
         <v>1161</v>
       </c>
       <c r="B1572" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1572" s="39" t="s">
-        <v>1162</v>
+        <v>22</v>
+      </c>
+      <c r="E1572" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1573" spans="1:5">
@@ -37688,21 +37686,21 @@
         <v>1161</v>
       </c>
       <c r="B1573" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1573" s="39">
-        <v>44320</v>
+        <v>27</v>
+      </c>
+      <c r="C1573" s="39" t="s">
+        <v>1162</v>
       </c>
     </row>
     <row r="1574" spans="1:5">
       <c r="A1574" s="39" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="B1574" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1574" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1574" s="39">
+        <v>44320</v>
       </c>
     </row>
     <row r="1575" spans="1:5">
@@ -37710,10 +37708,10 @@
         <v>1163</v>
       </c>
       <c r="B1575" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1575" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1576" spans="1:5">
@@ -37721,10 +37719,10 @@
         <v>1163</v>
       </c>
       <c r="B1576" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1576" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1577" spans="1:5">
@@ -37732,10 +37730,10 @@
         <v>1163</v>
       </c>
       <c r="B1577" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1577" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1578" spans="1:5">
@@ -37743,10 +37741,10 @@
         <v>1163</v>
       </c>
       <c r="B1578" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1578" s="39" t="s">
-        <v>1162</v>
+        <v>22</v>
+      </c>
+      <c r="E1578" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1579" spans="1:5">
@@ -37754,21 +37752,21 @@
         <v>1163</v>
       </c>
       <c r="B1579" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1579" s="39" t="s">
-        <v>1159</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1580" spans="1:5">
       <c r="A1580" s="39" t="s">
-        <v>1176</v>
+        <v>1163</v>
       </c>
       <c r="B1580" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1580" s="39" t="s">
-        <v>37</v>
+        <v>89</v>
+      </c>
+      <c r="C1580" s="39" t="s">
+        <v>1159</v>
       </c>
     </row>
     <row r="1581" spans="1:5">
@@ -37776,10 +37774,10 @@
         <v>1176</v>
       </c>
       <c r="B1581" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1581" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1582" spans="1:5">
@@ -37787,10 +37785,10 @@
         <v>1176</v>
       </c>
       <c r="B1582" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1582" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1583" spans="1:5">
@@ -37798,10 +37796,10 @@
         <v>1176</v>
       </c>
       <c r="B1583" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1583" s="39" t="s">
-        <v>1177</v>
+        <v>95</v>
+      </c>
+      <c r="E1583" s="39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="1584" spans="1:5">
@@ -37809,10 +37807,10 @@
         <v>1176</v>
       </c>
       <c r="B1584" s="39" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C1584" s="39" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="1585" spans="1:5">
@@ -37820,10 +37818,10 @@
         <v>1176</v>
       </c>
       <c r="B1585" s="39" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C1585" s="39" t="s">
-        <v>1169</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1586" spans="1:5">
@@ -37831,21 +37829,21 @@
         <v>1176</v>
       </c>
       <c r="B1586" s="39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C1586" s="39" t="s">
-        <v>1179</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1587" spans="1:5">
       <c r="A1587" s="39" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="B1587" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1587" s="39" t="s">
-        <v>37</v>
+        <v>106</v>
+      </c>
+      <c r="C1587" s="39" t="s">
+        <v>1179</v>
       </c>
     </row>
     <row r="1588" spans="1:5">
@@ -37853,10 +37851,10 @@
         <v>1180</v>
       </c>
       <c r="B1588" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1588" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1589" spans="1:5">
@@ -37864,10 +37862,10 @@
         <v>1180</v>
       </c>
       <c r="B1589" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1589" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1590" spans="1:5">
@@ -37875,10 +37873,10 @@
         <v>1180</v>
       </c>
       <c r="B1590" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1590" s="39" t="s">
-        <v>1181</v>
+        <v>95</v>
+      </c>
+      <c r="E1590" s="39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="1591" spans="1:5">
@@ -37886,10 +37884,10 @@
         <v>1180</v>
       </c>
       <c r="B1591" s="39" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C1591" s="39" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1592" spans="1:5">
@@ -37897,10 +37895,10 @@
         <v>1180</v>
       </c>
       <c r="B1592" s="39" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="C1592" s="39" t="s">
-        <v>1167</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1593" spans="1:5">
@@ -37908,21 +37906,21 @@
         <v>1180</v>
       </c>
       <c r="B1593" s="39" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C1593" s="39" t="s">
-        <v>1179</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="1594" spans="1:5">
       <c r="A1594" s="39" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="B1594" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1594" s="39" t="s">
-        <v>37</v>
+        <v>106</v>
+      </c>
+      <c r="C1594" s="39" t="s">
+        <v>1179</v>
       </c>
     </row>
     <row r="1595" spans="1:5">
@@ -37930,10 +37928,10 @@
         <v>1183</v>
       </c>
       <c r="B1595" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1595" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1596" spans="1:5">
@@ -37941,10 +37939,10 @@
         <v>1183</v>
       </c>
       <c r="B1596" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1596" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1597" spans="1:5">
@@ -37952,10 +37950,10 @@
         <v>1183</v>
       </c>
       <c r="B1597" s="39" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E1597" s="39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="1598" spans="1:5">
@@ -37963,10 +37961,10 @@
         <v>1183</v>
       </c>
       <c r="B1598" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1598" s="39" t="s">
-        <v>1010</v>
+        <v>22</v>
+      </c>
+      <c r="E1598" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1599" spans="1:5">
@@ -37974,10 +37972,10 @@
         <v>1183</v>
       </c>
       <c r="B1599" s="39" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="C1599" s="39" t="s">
-        <v>387</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="1600" spans="1:5">
@@ -37985,10 +37983,10 @@
         <v>1183</v>
       </c>
       <c r="B1600" s="39" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C1600" s="39" t="s">
-        <v>172</v>
+        <v>387</v>
       </c>
     </row>
     <row r="1601" spans="1:5">
@@ -37996,21 +37994,21 @@
         <v>1183</v>
       </c>
       <c r="B1601" s="39" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C1601" s="39" t="s">
-        <v>1047</v>
+        <v>172</v>
       </c>
     </row>
     <row r="1602" spans="1:5">
       <c r="A1602" s="39" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B1602" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1602" s="39" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="C1602" s="39" t="s">
+        <v>1047</v>
       </c>
     </row>
     <row r="1603" spans="1:5">
@@ -38018,10 +38016,10 @@
         <v>1184</v>
       </c>
       <c r="B1603" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1603" s="39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1604" spans="1:5">
@@ -38029,10 +38027,10 @@
         <v>1184</v>
       </c>
       <c r="B1604" s="39" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E1604" s="39" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="1605" spans="1:5">
@@ -38040,10 +38038,10 @@
         <v>1184</v>
       </c>
       <c r="B1605" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1605" s="39" t="s">
-        <v>1012</v>
+        <v>95</v>
+      </c>
+      <c r="E1605" s="39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="1606" spans="1:5">
@@ -38051,10 +38049,10 @@
         <v>1184</v>
       </c>
       <c r="B1606" s="39" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1606" s="39" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="1607" spans="1:5">
@@ -38062,10 +38060,10 @@
         <v>1184</v>
       </c>
       <c r="B1607" s="39" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C1607" s="39" t="s">
-        <v>260</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="1608" spans="1:5">
@@ -38073,10 +38071,10 @@
         <v>1184</v>
       </c>
       <c r="B1608" s="39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C1608" s="39" t="s">
-        <v>172</v>
+        <v>260</v>
       </c>
     </row>
     <row r="1609" spans="1:5">
@@ -38084,14 +38082,25 @@
         <v>1184</v>
       </c>
       <c r="B1609" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1609" s="39" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:5">
+      <c r="A1610" s="39" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B1610" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C1609" s="39" t="s">
+      <c r="C1610" s="39" t="s">
         <v>387</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1609" xr:uid="{32A0A4D2-FA49-40AB-B76A-75F48EB88A9F}"/>
+  <autoFilter ref="A1:F1610" xr:uid="{32A0A4D2-FA49-40AB-B76A-75F48EB88A9F}"/>
   <conditionalFormatting sqref="A1100">
     <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Changed report generation file path
</commit_message>
<xml_diff>
--- a/PartnerMasterConfiguration.xlsx
+++ b/PartnerMasterConfiguration.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0234BECF-6939-4C85-827F-724BB9FEB645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710DBA3F-CA2F-4502-8059-A155192D8F70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7726" uniqueCount="1186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7726" uniqueCount="1188">
   <si>
     <t>Partner ID</t>
   </si>
@@ -3680,6 +3680,12 @@
   </si>
   <si>
     <t>alen@bomisco.com;rajesh@bomisco.com;govinda@bomisco.com;doris@bomisco.com;mihir@bomisco.com;bhavya@bomisco.com;janani@bomisco.com;palak@bomisco.com;lohith@bomisco.com;shivangi@bomisco.com;satish@bomisco.com;lohith@bomisco.com</t>
+  </si>
+  <si>
+    <t>D:\ArloVerisure\Source\&lt;Partner ID&gt;\&lt;POS_Inventory_Flag&gt;\DDMMYY\Original\&lt;original_file_name&gt;</t>
+  </si>
+  <si>
+    <t>D:\ArloVerisure\Transformed\&lt;Partner ID&gt;\&lt;POS_Inventory_Flag&gt;\DDMMYY\&lt;renamed_file&gt;</t>
   </si>
 </sst>
 </file>
@@ -4708,10 +4714,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="A190" sqref="A190"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2:K167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4860,10 +4866,10 @@
         <v>398</v>
       </c>
       <c r="J2" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K2" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L2" s="60" t="s">
         <v>65</v>
@@ -4934,10 +4940,10 @@
         <v>397</v>
       </c>
       <c r="J3" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K3" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L3" s="60" t="s">
         <v>66</v>
@@ -5008,10 +5014,10 @@
         <v>397</v>
       </c>
       <c r="J4" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K4" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L4" s="60" t="s">
         <v>1</v>
@@ -5082,10 +5088,10 @@
         <v>398</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K5" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L5" s="60" t="s">
         <v>67</v>
@@ -5156,10 +5162,10 @@
         <v>401</v>
       </c>
       <c r="J6" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K6" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L6" s="60" t="s">
         <v>121</v>
@@ -5230,10 +5236,10 @@
         <v>401</v>
       </c>
       <c r="J7" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K7" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L7" s="60" t="s">
         <v>123</v>
@@ -5304,10 +5310,10 @@
         <v>406</v>
       </c>
       <c r="J8" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K8" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L8" s="60" t="s">
         <v>203</v>
@@ -5378,10 +5384,10 @@
         <v>406</v>
       </c>
       <c r="J9" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K9" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L9" s="60" t="s">
         <v>215</v>
@@ -5452,10 +5458,10 @@
         <v>406</v>
       </c>
       <c r="J10" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K10" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L10" s="60" t="s">
         <v>285</v>
@@ -5532,10 +5538,10 @@
         <v>403</v>
       </c>
       <c r="J11" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K11" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L11" s="60" t="s">
         <v>301</v>
@@ -5610,10 +5616,10 @@
         <v>400</v>
       </c>
       <c r="J12" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K12" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L12" s="60" t="s">
         <v>325</v>
@@ -5686,10 +5692,10 @@
       </c>
       <c r="I13" s="60"/>
       <c r="J13" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K13" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L13" s="60" t="s">
         <v>416</v>
@@ -5754,10 +5760,10 @@
       </c>
       <c r="I14" s="60"/>
       <c r="J14" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K14" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L14" s="60" t="s">
         <v>345</v>
@@ -5820,10 +5826,10 @@
         <v>399</v>
       </c>
       <c r="J15" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K15" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>435</v>
@@ -5888,10 +5894,10 @@
         <v>399</v>
       </c>
       <c r="J16" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K16" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>436</v>
@@ -5956,10 +5962,10 @@
         <v>405</v>
       </c>
       <c r="J17" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K17" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>445</v>
@@ -6024,10 +6030,10 @@
         <v>405</v>
       </c>
       <c r="J18" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K18" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>446</v>
@@ -6092,10 +6098,10 @@
         <v>401</v>
       </c>
       <c r="J19" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K19" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>445</v>
@@ -6154,10 +6160,10 @@
         <v>401</v>
       </c>
       <c r="J20" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K20" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>446</v>
@@ -6216,10 +6222,10 @@
         <v>399</v>
       </c>
       <c r="J21" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K21" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>464</v>
@@ -6282,10 +6288,10 @@
         <v>399</v>
       </c>
       <c r="J22" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K22" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>111</v>
@@ -6345,10 +6351,10 @@
         <v>399</v>
       </c>
       <c r="J23" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K23" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>482</v>
@@ -6404,10 +6410,10 @@
         <v>405</v>
       </c>
       <c r="J24" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K24" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>345</v>
@@ -6467,10 +6473,10 @@
         <v>405</v>
       </c>
       <c r="J25" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K25" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>227</v>
@@ -6530,10 +6536,10 @@
         <v>405</v>
       </c>
       <c r="J26" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K26" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L26" s="60" t="s">
         <v>138</v>
@@ -6608,10 +6614,10 @@
         <v>401</v>
       </c>
       <c r="J27" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K27" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L27" s="60" t="s">
         <v>224</v>
@@ -6686,10 +6692,10 @@
         <v>401</v>
       </c>
       <c r="J28" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K28" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>504</v>
@@ -6754,10 +6760,10 @@
         <v>401</v>
       </c>
       <c r="J29" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K29" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L29" s="60" t="s">
         <v>68</v>
@@ -6828,10 +6834,10 @@
         <v>401</v>
       </c>
       <c r="J30" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K30" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L30" s="60" t="s">
         <v>222</v>
@@ -6902,10 +6908,10 @@
         <v>405</v>
       </c>
       <c r="J31" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K31" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>513</v>
@@ -6967,10 +6973,10 @@
         <v>405</v>
       </c>
       <c r="J32" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K32" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>522</v>
@@ -7033,10 +7039,10 @@
         <v>405</v>
       </c>
       <c r="J33" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K33" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>526</v>
@@ -7099,10 +7105,10 @@
         <v>405</v>
       </c>
       <c r="J34" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K34" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>192</v>
@@ -7163,10 +7169,10 @@
         <v>405</v>
       </c>
       <c r="J35" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K35" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>531</v>
@@ -7222,10 +7228,10 @@
         <v>402</v>
       </c>
       <c r="J36" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K36" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L36" s="8" t="s">
         <v>126</v>
@@ -7286,10 +7292,10 @@
         <v>404</v>
       </c>
       <c r="J37" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K37" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L37" s="8" t="s">
         <v>135</v>
@@ -7350,10 +7356,10 @@
         <v>404</v>
       </c>
       <c r="J38" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K38" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L38" s="8" t="s">
         <v>136</v>
@@ -7414,10 +7420,10 @@
         <v>541</v>
       </c>
       <c r="J39" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K39" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>542</v>
@@ -7480,10 +7486,10 @@
         <v>541</v>
       </c>
       <c r="J40" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K40" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>543</v>
@@ -7546,10 +7552,10 @@
         <v>399</v>
       </c>
       <c r="J41" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K41" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>552</v>
@@ -7612,10 +7618,10 @@
         <v>399</v>
       </c>
       <c r="J42" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K42" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>553</v>
@@ -7678,10 +7684,10 @@
         <v>401</v>
       </c>
       <c r="J43" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K43" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>138</v>
@@ -7746,10 +7752,10 @@
         <v>405</v>
       </c>
       <c r="J44" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K44" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>561</v>
@@ -7812,10 +7818,10 @@
         <v>405</v>
       </c>
       <c r="J45" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K45" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L45" s="8" t="s">
         <v>562</v>
@@ -7878,10 +7884,10 @@
         <v>401</v>
       </c>
       <c r="J46" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K46" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L46" s="8" t="s">
         <v>568</v>
@@ -7946,10 +7952,10 @@
         <v>399</v>
       </c>
       <c r="J47" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K47" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L47" s="8" t="s">
         <v>572</v>
@@ -8014,10 +8020,10 @@
         <v>399</v>
       </c>
       <c r="J48" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K48" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L48" s="8" t="s">
         <v>573</v>
@@ -8082,10 +8088,10 @@
         <v>405</v>
       </c>
       <c r="J49" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K49" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>568</v>
@@ -8146,10 +8152,10 @@
         <v>399</v>
       </c>
       <c r="J50" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K50" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L50" s="8" t="s">
         <v>297</v>
@@ -8210,10 +8216,10 @@
         <v>401</v>
       </c>
       <c r="J51" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K51" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L51" s="8" t="s">
         <v>590</v>
@@ -8278,10 +8284,10 @@
         <v>599</v>
       </c>
       <c r="J52" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K52" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L52" s="8" t="s">
         <v>600</v>
@@ -8346,10 +8352,10 @@
         <v>401</v>
       </c>
       <c r="J53" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K53" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L53" s="8" t="s">
         <v>107</v>
@@ -8407,10 +8413,10 @@
         <v>401</v>
       </c>
       <c r="J54" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K54" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L54" s="8" t="s">
         <v>16</v>
@@ -8468,10 +8474,10 @@
         <v>599</v>
       </c>
       <c r="J55" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K55" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>107</v>
@@ -8534,10 +8540,10 @@
         <v>599</v>
       </c>
       <c r="J56" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K56" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L56" s="8" t="s">
         <v>16</v>
@@ -8600,10 +8606,10 @@
         <v>399</v>
       </c>
       <c r="J57" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K57" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L57" s="8" t="s">
         <v>107</v>
@@ -8666,10 +8672,10 @@
         <v>399</v>
       </c>
       <c r="J58" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K58" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L58" s="8" t="s">
         <v>16</v>
@@ -8732,10 +8738,10 @@
         <v>399</v>
       </c>
       <c r="J59" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K59" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L59" s="8" t="s">
         <v>445</v>
@@ -8798,10 +8804,10 @@
         <v>399</v>
       </c>
       <c r="J60" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K60" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L60" s="8" t="s">
         <v>615</v>
@@ -8864,10 +8870,10 @@
         <v>399</v>
       </c>
       <c r="J61" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K61" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L61" s="8" t="s">
         <v>619</v>
@@ -8930,10 +8936,10 @@
         <v>399</v>
       </c>
       <c r="J62" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K62" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L62" s="8" t="s">
         <v>621</v>
@@ -8996,10 +9002,10 @@
         <v>399</v>
       </c>
       <c r="J63" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K63" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L63" s="8" t="s">
         <v>625</v>
@@ -9062,10 +9068,10 @@
         <v>399</v>
       </c>
       <c r="J64" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K64" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L64" s="8" t="s">
         <v>627</v>
@@ -9128,10 +9134,10 @@
         <v>399</v>
       </c>
       <c r="J65" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K65" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L65" s="8" t="s">
         <v>629</v>
@@ -9194,10 +9200,10 @@
         <v>401</v>
       </c>
       <c r="J66" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K66" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L66" s="8" t="s">
         <v>639</v>
@@ -9262,10 +9268,10 @@
         <v>399</v>
       </c>
       <c r="J67" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K67" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L67" s="8" t="s">
         <v>646</v>
@@ -9328,10 +9334,10 @@
         <v>654</v>
       </c>
       <c r="J68" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K68" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L68" s="8" t="s">
         <v>68</v>
@@ -9394,10 +9400,10 @@
         <v>654</v>
       </c>
       <c r="J69" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K69" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L69" s="8" t="s">
         <v>656</v>
@@ -9460,10 +9466,10 @@
         <v>399</v>
       </c>
       <c r="J70" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K70" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L70" s="8" t="s">
         <v>646</v>
@@ -9526,10 +9532,10 @@
         <v>401</v>
       </c>
       <c r="J71" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K71" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L71" s="8" t="s">
         <v>135</v>
@@ -9596,10 +9602,10 @@
         <v>401</v>
       </c>
       <c r="J72" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K72" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L72" s="8" t="s">
         <v>311</v>
@@ -9666,10 +9672,10 @@
         <v>399</v>
       </c>
       <c r="J73" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K73" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L73" s="8" t="s">
         <v>68</v>
@@ -9730,10 +9736,10 @@
         <v>399</v>
       </c>
       <c r="J74" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K74" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L74" s="8" t="s">
         <v>674</v>
@@ -9794,10 +9800,10 @@
         <v>399</v>
       </c>
       <c r="J75" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K75" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L75" s="8" t="s">
         <v>445</v>
@@ -9860,10 +9866,10 @@
         <v>399</v>
       </c>
       <c r="J76" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K76" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L76" s="8" t="s">
         <v>188</v>
@@ -9926,10 +9932,10 @@
         <v>401</v>
       </c>
       <c r="J77" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K77" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L77" s="8" t="s">
         <v>498</v>
@@ -9996,10 +10002,10 @@
         <v>722</v>
       </c>
       <c r="J78" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K78" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L78" s="8" t="s">
         <v>69</v>
@@ -10062,10 +10068,10 @@
         <v>725</v>
       </c>
       <c r="J79" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K79" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L79" s="8" t="s">
         <v>69</v>
@@ -10128,10 +10134,10 @@
         <v>405</v>
       </c>
       <c r="J80" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K80" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L80" s="8" t="s">
         <v>69</v>
@@ -10194,10 +10200,10 @@
         <v>399</v>
       </c>
       <c r="J81" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K81" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L81" s="8" t="s">
         <v>69</v>
@@ -10260,10 +10266,10 @@
         <v>399</v>
       </c>
       <c r="J82" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K82" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L82" s="8" t="s">
         <v>69</v>
@@ -10326,10 +10332,10 @@
         <v>399</v>
       </c>
       <c r="J83" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K83" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L83" s="8" t="s">
         <v>69</v>
@@ -10392,10 +10398,10 @@
         <v>541</v>
       </c>
       <c r="J84" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K84" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L84" s="8" t="s">
         <v>737</v>
@@ -10458,10 +10464,10 @@
         <v>541</v>
       </c>
       <c r="J85" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K85" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L85" s="8" t="s">
         <v>739</v>
@@ -10524,10 +10530,10 @@
         <v>747</v>
       </c>
       <c r="J86" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K86" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L86" s="8" t="s">
         <v>68</v>
@@ -10588,10 +10594,10 @@
         <v>747</v>
       </c>
       <c r="J87" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K87" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L87" s="8"/>
       <c r="M87" s="8" t="s">
@@ -10652,10 +10658,10 @@
         <v>399</v>
       </c>
       <c r="J88" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K88" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L88" s="8" t="s">
         <v>69</v>
@@ -10718,10 +10724,10 @@
         <v>399</v>
       </c>
       <c r="J89" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K89" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L89" s="8" t="s">
         <v>69</v>
@@ -10784,10 +10790,10 @@
         <v>401</v>
       </c>
       <c r="J90" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K90" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L90" s="8" t="s">
         <v>69</v>
@@ -10850,10 +10856,10 @@
         <v>599</v>
       </c>
       <c r="J91" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K91" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L91" s="8" t="s">
         <v>69</v>
@@ -10916,10 +10922,10 @@
         <v>401</v>
       </c>
       <c r="J92" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K92" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L92" s="8" t="s">
         <v>69</v>
@@ -10982,10 +10988,10 @@
         <v>599</v>
       </c>
       <c r="J93" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K93" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L93" s="8" t="s">
         <v>69</v>
@@ -11048,10 +11054,10 @@
         <v>399</v>
       </c>
       <c r="J94" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K94" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L94" s="8" t="s">
         <v>69</v>
@@ -11114,10 +11120,10 @@
         <v>763</v>
       </c>
       <c r="J95" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K95" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L95" s="8" t="s">
         <v>69</v>
@@ -11180,10 +11186,10 @@
         <v>399</v>
       </c>
       <c r="J96" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K96" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L96" s="8" t="s">
         <v>69</v>
@@ -11246,10 +11252,10 @@
         <v>399</v>
       </c>
       <c r="J97" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K97" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L97" s="8" t="s">
         <v>69</v>
@@ -11312,10 +11318,10 @@
         <v>399</v>
       </c>
       <c r="J98" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K98" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L98" s="8" t="s">
         <v>69</v>
@@ -11378,10 +11384,10 @@
         <v>401</v>
       </c>
       <c r="J99" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K99" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L99" s="8" t="s">
         <v>69</v>
@@ -11444,10 +11450,10 @@
         <v>399</v>
       </c>
       <c r="J100" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K100" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L100" s="8" t="s">
         <v>69</v>
@@ -11510,10 +11516,10 @@
         <v>399</v>
       </c>
       <c r="J101" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K101" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L101" s="8" t="s">
         <v>69</v>
@@ -11576,10 +11582,10 @@
         <v>399</v>
       </c>
       <c r="J102" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K102" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L102" s="8" t="s">
         <v>69</v>
@@ -11642,10 +11648,10 @@
         <v>399</v>
       </c>
       <c r="J103" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K103" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L103" s="8" t="s">
         <v>69</v>
@@ -11708,10 +11714,10 @@
         <v>399</v>
       </c>
       <c r="J104" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K104" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L104" s="8" t="s">
         <v>69</v>
@@ -11774,10 +11780,10 @@
         <v>401</v>
       </c>
       <c r="J105" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K105" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L105" s="8" t="s">
         <v>69</v>
@@ -11840,10 +11846,10 @@
         <v>399</v>
       </c>
       <c r="J106" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K106" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L106" s="8" t="s">
         <v>69</v>
@@ -11906,10 +11912,10 @@
         <v>399</v>
       </c>
       <c r="J107" s="60" t="s">
-        <v>410</v>
+        <v>1186</v>
       </c>
       <c r="K107" s="60" t="s">
-        <v>411</v>
+        <v>1187</v>
       </c>
       <c r="L107" s="8" t="s">
         <v>69</v>
@@ -11971,11 +11977,11 @@
       <c r="I108" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="J108" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K108" s="27" t="s">
-        <v>411</v>
+      <c r="J108" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K108" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L108" s="27" t="s">
         <v>63</v>
@@ -12039,11 +12045,11 @@
       <c r="I109" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="J109" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K109" s="27" t="s">
-        <v>411</v>
+      <c r="J109" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K109" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L109" s="27" t="s">
         <v>64</v>
@@ -12107,11 +12113,11 @@
       <c r="I110" s="27" t="s">
         <v>409</v>
       </c>
-      <c r="J110" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K110" s="27" t="s">
-        <v>411</v>
+      <c r="J110" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K110" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L110" s="27" t="s">
         <v>135</v>
@@ -12175,11 +12181,11 @@
       <c r="I111" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="J111" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K111" s="27" t="s">
-        <v>411</v>
+      <c r="J111" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K111" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L111" s="27" t="s">
         <v>372</v>
@@ -12249,11 +12255,11 @@
       <c r="I112" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="J112" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K112" s="27" t="s">
-        <v>411</v>
+      <c r="J112" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K112" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L112" s="27" t="s">
         <v>142</v>
@@ -12317,11 +12323,11 @@
       <c r="I113" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="J113" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K113" s="27" t="s">
-        <v>411</v>
+      <c r="J113" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K113" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L113" s="27" t="s">
         <v>311</v>
@@ -12391,11 +12397,11 @@
       <c r="I114" s="27" t="s">
         <v>400</v>
       </c>
-      <c r="J114" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K114" s="27" t="s">
-        <v>411</v>
+      <c r="J114" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K114" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L114" s="27" t="s">
         <v>294</v>
@@ -12468,11 +12474,11 @@
       <c r="I115" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="J115" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K115" s="27" t="s">
-        <v>411</v>
+      <c r="J115" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K115" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L115" s="27" t="s">
         <v>316</v>
@@ -12545,11 +12551,11 @@
       <c r="I116" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="J116" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K116" s="27" t="s">
-        <v>411</v>
+      <c r="J116" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K116" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L116" s="27" t="s">
         <v>259</v>
@@ -12613,11 +12619,11 @@
       <c r="I117" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="J117" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K117" s="27" t="s">
-        <v>411</v>
+      <c r="J117" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K117" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L117" s="27" t="s">
         <v>260</v>
@@ -12681,11 +12687,11 @@
       <c r="I118" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="J118" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K118" s="27" t="s">
-        <v>411</v>
+      <c r="J118" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K118" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L118" s="27" t="s">
         <v>253</v>
@@ -12755,11 +12761,11 @@
       <c r="H119" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J119" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K119" s="27" t="s">
-        <v>411</v>
+      <c r="J119" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K119" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L119" s="27" t="s">
         <v>445</v>
@@ -12811,11 +12817,11 @@
       <c r="H120" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J120" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K120" s="27" t="s">
-        <v>411</v>
+      <c r="J120" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K120" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L120" s="27" t="s">
         <v>803</v>
@@ -12867,11 +12873,11 @@
       <c r="H121" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J121" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K121" s="27" t="s">
-        <v>411</v>
+      <c r="J121" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K121" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L121" s="71" t="s">
         <v>445</v>
@@ -12923,11 +12929,11 @@
       <c r="H122" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J122" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K122" s="27" t="s">
-        <v>411</v>
+      <c r="J122" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K122" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L122" s="71" t="s">
         <v>803</v>
@@ -12979,11 +12985,11 @@
       <c r="H123" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J123" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K123" s="27" t="s">
-        <v>411</v>
+      <c r="J123" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K123" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L123" s="71" t="s">
         <v>445</v>
@@ -13035,11 +13041,11 @@
       <c r="H124" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J124" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K124" s="27" t="s">
-        <v>411</v>
+      <c r="J124" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K124" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L124" s="71" t="s">
         <v>445</v>
@@ -13091,11 +13097,11 @@
       <c r="H125" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J125" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K125" s="27" t="s">
-        <v>411</v>
+      <c r="J125" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K125" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L125" s="27" t="s">
         <v>445</v>
@@ -13147,11 +13153,11 @@
       <c r="H126" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J126" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K126" s="27" t="s">
-        <v>411</v>
+      <c r="J126" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K126" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L126" s="27" t="s">
         <v>803</v>
@@ -13203,11 +13209,11 @@
       <c r="H127" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J127" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K127" s="27" t="s">
-        <v>411</v>
+      <c r="J127" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K127" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L127" s="71" t="s">
         <v>445</v>
@@ -13259,11 +13265,11 @@
       <c r="H128" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J128" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K128" s="27" t="s">
-        <v>411</v>
+      <c r="J128" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K128" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L128" s="71" t="s">
         <v>445</v>
@@ -13315,11 +13321,11 @@
       <c r="H129" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J129" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K129" s="27" t="s">
-        <v>411</v>
+      <c r="J129" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K129" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L129" s="27" t="s">
         <v>445</v>
@@ -13371,11 +13377,11 @@
       <c r="H130" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J130" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K130" s="27" t="s">
-        <v>411</v>
+      <c r="J130" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K130" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L130" s="27" t="s">
         <v>803</v>
@@ -13427,11 +13433,11 @@
       <c r="H131" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J131" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K131" s="27" t="s">
-        <v>411</v>
+      <c r="J131" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K131" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L131" s="69" t="s">
         <v>826</v>
@@ -13483,11 +13489,11 @@
       <c r="H132" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J132" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K132" s="27" t="s">
-        <v>411</v>
+      <c r="J132" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K132" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L132" s="69" t="s">
         <v>260</v>
@@ -13539,11 +13545,11 @@
       <c r="H133" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J133" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K133" s="27" t="s">
-        <v>411</v>
+      <c r="J133" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K133" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L133" s="71" t="s">
         <v>832</v>
@@ -13596,11 +13602,11 @@
       <c r="H134" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J134" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K134" s="27" t="s">
-        <v>411</v>
+      <c r="J134" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K134" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L134" s="27" t="s">
         <v>833</v>
@@ -13652,11 +13658,11 @@
       <c r="H135" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J135" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K135" s="27" t="s">
-        <v>411</v>
+      <c r="J135" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K135" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L135" s="27" t="s">
         <v>838</v>
@@ -13714,11 +13720,11 @@
       <c r="H136" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J136" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K136" s="27" t="s">
-        <v>411</v>
+      <c r="J136" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K136" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L136" s="27" t="s">
         <v>260</v>
@@ -13770,11 +13776,11 @@
       <c r="H137" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J137" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K137" s="27" t="s">
-        <v>411</v>
+      <c r="J137" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K137" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L137" s="34" t="s">
         <v>843</v>
@@ -13832,11 +13838,11 @@
       <c r="H138" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J138" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K138" s="27" t="s">
-        <v>411</v>
+      <c r="J138" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K138" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L138" s="74" t="s">
         <v>197</v>
@@ -13891,11 +13897,11 @@
       <c r="H139" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J139" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K139" s="27" t="s">
-        <v>411</v>
+      <c r="J139" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K139" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L139" s="27" t="s">
         <v>851</v>
@@ -13953,11 +13959,11 @@
       <c r="H140" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J140" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K140" s="27" t="s">
-        <v>411</v>
+      <c r="J140" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K140" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L140" s="27" t="s">
         <v>855</v>
@@ -14011,11 +14017,11 @@
       <c r="H141" s="76" t="s">
         <v>1185</v>
       </c>
-      <c r="J141" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="K141" s="27" t="s">
-        <v>411</v>
+      <c r="J141" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K141" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L141" s="27" t="s">
         <v>860</v>
@@ -14076,11 +14082,11 @@
       <c r="I142" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="J142" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K142" s="16" t="s">
-        <v>411</v>
+      <c r="J142" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K142" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L142" s="10" t="s">
         <v>939</v>
@@ -14151,11 +14157,11 @@
       <c r="I143" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J143" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K143" s="16" t="s">
-        <v>411</v>
+      <c r="J143" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K143" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L143" s="8" t="s">
         <v>445</v>
@@ -14222,11 +14228,11 @@
       <c r="I144" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J144" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K144" s="16" t="s">
-        <v>411</v>
+      <c r="J144" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K144" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L144" s="8" t="s">
         <v>944</v>
@@ -14293,11 +14299,11 @@
       <c r="I145" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J145" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K145" s="16" t="s">
-        <v>411</v>
+      <c r="J145" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K145" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L145" s="8" t="s">
         <v>264</v>
@@ -14364,11 +14370,11 @@
       <c r="I146" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J146" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K146" s="16" t="s">
-        <v>411</v>
+      <c r="J146" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K146" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L146" s="10" t="s">
         <v>265</v>
@@ -14435,11 +14441,11 @@
       <c r="I147" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="J147" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K147" s="16" t="s">
-        <v>411</v>
+      <c r="J147" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K147" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L147" s="8" t="s">
         <v>325</v>
@@ -14510,11 +14516,11 @@
       <c r="I148" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J148" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K148" s="16" t="s">
-        <v>411</v>
+      <c r="J148" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K148" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L148" s="8" t="s">
         <v>949</v>
@@ -14585,11 +14591,11 @@
       <c r="I149" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="J149" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K149" s="16" t="s">
-        <v>411</v>
+      <c r="J149" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K149" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L149" s="8" t="s">
         <v>954</v>
@@ -14663,11 +14669,11 @@
       <c r="I150" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="J150" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K150" s="16" t="s">
-        <v>411</v>
+      <c r="J150" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K150" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L150" s="8" t="s">
         <v>958</v>
@@ -14734,11 +14740,11 @@
       <c r="I151" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="J151" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K151" s="16" t="s">
-        <v>411</v>
+      <c r="J151" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K151" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L151" s="10" t="s">
         <v>962</v>
@@ -14805,11 +14811,11 @@
       <c r="I152" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="J152" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K152" s="16" t="s">
-        <v>411</v>
+      <c r="J152" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K152" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L152" s="8" t="s">
         <v>260</v>
@@ -14876,11 +14882,11 @@
       <c r="I153" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="J153" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K153" s="16" t="s">
-        <v>411</v>
+      <c r="J153" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K153" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L153" s="8" t="s">
         <v>325</v>
@@ -14951,11 +14957,11 @@
       <c r="I154" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J154" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K154" s="16" t="s">
-        <v>411</v>
+      <c r="J154" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K154" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L154" s="8" t="s">
         <v>126</v>
@@ -15022,11 +15028,11 @@
       <c r="I155" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J155" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K155" s="16" t="s">
-        <v>411</v>
+      <c r="J155" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K155" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L155" s="8" t="s">
         <v>132</v>
@@ -15093,11 +15099,11 @@
       <c r="I156" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="J156" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K156" s="16" t="s">
-        <v>411</v>
+      <c r="J156" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K156" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L156" s="8" t="s">
         <v>260</v>
@@ -15167,11 +15173,11 @@
       <c r="I157" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="J157" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K157" s="16" t="s">
-        <v>411</v>
+      <c r="J157" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K157" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L157" s="10" t="s">
         <v>969</v>
@@ -15245,11 +15251,11 @@
       <c r="I158" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="J158" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K158" s="16" t="s">
-        <v>411</v>
+      <c r="J158" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K158" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L158" s="8" t="s">
         <v>69</v>
@@ -15316,11 +15322,11 @@
       <c r="I159" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="J159" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K159" s="16" t="s">
-        <v>411</v>
+      <c r="J159" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K159" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L159" s="10" t="s">
         <v>70</v>
@@ -15387,11 +15393,11 @@
       <c r="I160" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="J160" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K160" s="16" t="s">
-        <v>411</v>
+      <c r="J160" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K160" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L160" s="8" t="s">
         <v>69</v>
@@ -15458,11 +15464,11 @@
       <c r="I161" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="J161" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K161" s="16" t="s">
-        <v>411</v>
+      <c r="J161" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K161" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L161" s="10" t="s">
         <v>70</v>
@@ -15529,11 +15535,11 @@
       <c r="I162" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J162" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K162" s="16" t="s">
-        <v>411</v>
+      <c r="J162" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K162" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L162" s="8" t="s">
         <v>68</v>
@@ -15600,11 +15606,11 @@
       <c r="I163" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J163" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K163" s="16" t="s">
-        <v>411</v>
+      <c r="J163" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K163" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L163" s="10" t="s">
         <v>979</v>
@@ -15671,11 +15677,11 @@
       <c r="I164" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="J164" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K164" s="16" t="s">
-        <v>411</v>
+      <c r="J164" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K164" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L164" s="16" t="s">
         <v>1046</v>
@@ -15730,11 +15736,11 @@
       <c r="I165" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="J165" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K165" s="16" t="s">
-        <v>411</v>
+      <c r="J165" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K165" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L165" s="16" t="s">
         <v>118</v>
@@ -15789,11 +15795,11 @@
       <c r="I166" s="16" t="s">
         <v>407</v>
       </c>
-      <c r="J166" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K166" s="16" t="s">
-        <v>411</v>
+      <c r="J166" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K166" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L166" s="16" t="s">
         <v>305</v>
@@ -15848,11 +15854,11 @@
       <c r="I167" s="16" t="s">
         <v>407</v>
       </c>
-      <c r="J167" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="K167" s="16" t="s">
-        <v>411</v>
+      <c r="J167" s="60" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K167" s="60" t="s">
+        <v>1187</v>
       </c>
       <c r="L167" s="16" t="s">
         <v>307</v>

</xml_diff>

<commit_message>
Change Report genertion file path
</commit_message>
<xml_diff>
--- a/PartnerMasterConfiguration.xlsx
+++ b/PartnerMasterConfiguration.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AE7CF5-FEB3-4826-BAD5-B6B5D9F9F93A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0431B21D-993D-4A5F-904D-558EB79FECC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7713" uniqueCount="1184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7713" uniqueCount="1186">
   <si>
     <t>Partner ID</t>
   </si>
@@ -3674,6 +3674,12 @@
   </si>
   <si>
     <t>VAT Nr.</t>
+  </si>
+  <si>
+    <t>D:\ArloVerisure\Source\&lt;Partner ID&gt;\&lt;POS_Inventory_Flag&gt;\DDMMYY\Original\&lt;original_file_name&gt;</t>
+  </si>
+  <si>
+    <t>D:\ArloVerisure\Transformed\&lt;Partner ID&gt;\&lt;POS_Inventory_Flag&gt;\DDMMYY\&lt;renamed_file&gt;</t>
   </si>
 </sst>
 </file>
@@ -4291,10 +4297,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -4713,10 +4719,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2:K167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4865,10 +4871,10 @@
         <v>397</v>
       </c>
       <c r="J2" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K2" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L2" s="60" t="s">
         <v>65</v>
@@ -4939,10 +4945,10 @@
         <v>396</v>
       </c>
       <c r="J3" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K3" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L3" s="60" t="s">
         <v>66</v>
@@ -4994,7 +5000,7 @@
       <c r="C4" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="82" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="60" t="s">
@@ -5013,10 +5019,10 @@
         <v>396</v>
       </c>
       <c r="J4" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K4" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L4" s="60" t="s">
         <v>1</v>
@@ -5087,10 +5093,10 @@
         <v>397</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K5" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L5" s="60" t="s">
         <v>67</v>
@@ -5161,10 +5167,10 @@
         <v>400</v>
       </c>
       <c r="J6" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K6" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L6" s="60" t="s">
         <v>121</v>
@@ -5235,10 +5241,10 @@
         <v>400</v>
       </c>
       <c r="J7" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K7" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L7" s="60" t="s">
         <v>123</v>
@@ -5309,10 +5315,10 @@
         <v>405</v>
       </c>
       <c r="J8" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K8" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L8" s="60" t="s">
         <v>202</v>
@@ -5383,10 +5389,10 @@
         <v>405</v>
       </c>
       <c r="J9" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K9" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L9" s="60" t="s">
         <v>214</v>
@@ -5457,10 +5463,10 @@
         <v>405</v>
       </c>
       <c r="J10" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K10" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L10" s="60" t="s">
         <v>284</v>
@@ -5537,10 +5543,10 @@
         <v>402</v>
       </c>
       <c r="J11" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K11" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L11" s="60" t="s">
         <v>300</v>
@@ -5615,10 +5621,10 @@
         <v>399</v>
       </c>
       <c r="J12" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K12" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L12" s="60" t="s">
         <v>324</v>
@@ -5691,10 +5697,10 @@
       </c>
       <c r="I13" s="60"/>
       <c r="J13" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K13" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L13" s="60" t="s">
         <v>415</v>
@@ -5759,10 +5765,10 @@
       </c>
       <c r="I14" s="60"/>
       <c r="J14" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K14" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L14" s="60" t="s">
         <v>344</v>
@@ -5825,10 +5831,10 @@
         <v>398</v>
       </c>
       <c r="J15" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K15" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>434</v>
@@ -5893,10 +5899,10 @@
         <v>398</v>
       </c>
       <c r="J16" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K16" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>435</v>
@@ -5961,10 +5967,10 @@
         <v>404</v>
       </c>
       <c r="J17" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K17" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>444</v>
@@ -6029,10 +6035,10 @@
         <v>404</v>
       </c>
       <c r="J18" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K18" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>445</v>
@@ -6097,10 +6103,10 @@
         <v>400</v>
       </c>
       <c r="J19" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K19" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>444</v>
@@ -6159,10 +6165,10 @@
         <v>400</v>
       </c>
       <c r="J20" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K20" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>445</v>
@@ -6221,10 +6227,10 @@
         <v>398</v>
       </c>
       <c r="J21" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K21" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>463</v>
@@ -6287,10 +6293,10 @@
         <v>398</v>
       </c>
       <c r="J22" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K22" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>111</v>
@@ -6350,10 +6356,10 @@
         <v>398</v>
       </c>
       <c r="J23" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K23" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>481</v>
@@ -6409,10 +6415,10 @@
         <v>404</v>
       </c>
       <c r="J24" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K24" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>344</v>
@@ -6472,10 +6478,10 @@
         <v>404</v>
       </c>
       <c r="J25" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K25" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>226</v>
@@ -6535,10 +6541,10 @@
         <v>404</v>
       </c>
       <c r="J26" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K26" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L26" s="60" t="s">
         <v>138</v>
@@ -6613,10 +6619,10 @@
         <v>400</v>
       </c>
       <c r="J27" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K27" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L27" s="60" t="s">
         <v>223</v>
@@ -6691,10 +6697,10 @@
         <v>400</v>
       </c>
       <c r="J28" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K28" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>503</v>
@@ -6759,10 +6765,10 @@
         <v>400</v>
       </c>
       <c r="J29" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K29" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L29" s="60" t="s">
         <v>68</v>
@@ -6833,10 +6839,10 @@
         <v>400</v>
       </c>
       <c r="J30" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K30" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L30" s="60" t="s">
         <v>221</v>
@@ -6907,10 +6913,10 @@
         <v>404</v>
       </c>
       <c r="J31" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K31" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>512</v>
@@ -6972,10 +6978,10 @@
         <v>404</v>
       </c>
       <c r="J32" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K32" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>521</v>
@@ -7038,10 +7044,10 @@
         <v>404</v>
       </c>
       <c r="J33" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K33" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>525</v>
@@ -7104,10 +7110,10 @@
         <v>404</v>
       </c>
       <c r="J34" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K34" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>191</v>
@@ -7168,10 +7174,10 @@
         <v>404</v>
       </c>
       <c r="J35" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K35" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>530</v>
@@ -7227,10 +7233,10 @@
         <v>401</v>
       </c>
       <c r="J36" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K36" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L36" s="8" t="s">
         <v>126</v>
@@ -7291,10 +7297,10 @@
         <v>403</v>
       </c>
       <c r="J37" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K37" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L37" s="8" t="s">
         <v>135</v>
@@ -7355,10 +7361,10 @@
         <v>403</v>
       </c>
       <c r="J38" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K38" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L38" s="8" t="s">
         <v>136</v>
@@ -7419,10 +7425,10 @@
         <v>540</v>
       </c>
       <c r="J39" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K39" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>541</v>
@@ -7485,10 +7491,10 @@
         <v>540</v>
       </c>
       <c r="J40" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K40" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>542</v>
@@ -7551,10 +7557,10 @@
         <v>398</v>
       </c>
       <c r="J41" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K41" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>551</v>
@@ -7617,10 +7623,10 @@
         <v>398</v>
       </c>
       <c r="J42" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K42" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>552</v>
@@ -7683,10 +7689,10 @@
         <v>400</v>
       </c>
       <c r="J43" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K43" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>138</v>
@@ -7751,10 +7757,10 @@
         <v>404</v>
       </c>
       <c r="J44" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K44" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>560</v>
@@ -7817,10 +7823,10 @@
         <v>404</v>
       </c>
       <c r="J45" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K45" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L45" s="8" t="s">
         <v>561</v>
@@ -7883,10 +7889,10 @@
         <v>400</v>
       </c>
       <c r="J46" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K46" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L46" s="8" t="s">
         <v>567</v>
@@ -7951,10 +7957,10 @@
         <v>398</v>
       </c>
       <c r="J47" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K47" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L47" s="8" t="s">
         <v>571</v>
@@ -8019,10 +8025,10 @@
         <v>398</v>
       </c>
       <c r="J48" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K48" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L48" s="8" t="s">
         <v>572</v>
@@ -8087,10 +8093,10 @@
         <v>404</v>
       </c>
       <c r="J49" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K49" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>567</v>
@@ -8151,10 +8157,10 @@
         <v>398</v>
       </c>
       <c r="J50" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K50" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L50" s="8" t="s">
         <v>296</v>
@@ -8215,10 +8221,10 @@
         <v>400</v>
       </c>
       <c r="J51" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K51" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L51" s="8" t="s">
         <v>589</v>
@@ -8283,10 +8289,10 @@
         <v>598</v>
       </c>
       <c r="J52" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K52" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L52" s="8" t="s">
         <v>599</v>
@@ -8351,10 +8357,10 @@
         <v>400</v>
       </c>
       <c r="J53" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K53" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L53" s="8" t="s">
         <v>107</v>
@@ -8412,10 +8418,10 @@
         <v>400</v>
       </c>
       <c r="J54" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K54" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L54" s="8" t="s">
         <v>16</v>
@@ -8473,10 +8479,10 @@
         <v>598</v>
       </c>
       <c r="J55" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K55" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>107</v>
@@ -8539,10 +8545,10 @@
         <v>598</v>
       </c>
       <c r="J56" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K56" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L56" s="8" t="s">
         <v>16</v>
@@ -8605,10 +8611,10 @@
         <v>398</v>
       </c>
       <c r="J57" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K57" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L57" s="8" t="s">
         <v>107</v>
@@ -8671,10 +8677,10 @@
         <v>398</v>
       </c>
       <c r="J58" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K58" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L58" s="8" t="s">
         <v>16</v>
@@ -8737,10 +8743,10 @@
         <v>398</v>
       </c>
       <c r="J59" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K59" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L59" s="8" t="s">
         <v>444</v>
@@ -8803,10 +8809,10 @@
         <v>398</v>
       </c>
       <c r="J60" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K60" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L60" s="8" t="s">
         <v>614</v>
@@ -8869,10 +8875,10 @@
         <v>398</v>
       </c>
       <c r="J61" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K61" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L61" s="8" t="s">
         <v>618</v>
@@ -8935,10 +8941,10 @@
         <v>398</v>
       </c>
       <c r="J62" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K62" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L62" s="8" t="s">
         <v>620</v>
@@ -9001,10 +9007,10 @@
         <v>398</v>
       </c>
       <c r="J63" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K63" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L63" s="8" t="s">
         <v>624</v>
@@ -9067,10 +9073,10 @@
         <v>398</v>
       </c>
       <c r="J64" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K64" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L64" s="8" t="s">
         <v>626</v>
@@ -9133,10 +9139,10 @@
         <v>398</v>
       </c>
       <c r="J65" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K65" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L65" s="8" t="s">
         <v>628</v>
@@ -9199,10 +9205,10 @@
         <v>400</v>
       </c>
       <c r="J66" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K66" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L66" s="8" t="s">
         <v>638</v>
@@ -9267,10 +9273,10 @@
         <v>398</v>
       </c>
       <c r="J67" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K67" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L67" s="8" t="s">
         <v>645</v>
@@ -9333,10 +9339,10 @@
         <v>653</v>
       </c>
       <c r="J68" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K68" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L68" s="8" t="s">
         <v>68</v>
@@ -9399,10 +9405,10 @@
         <v>653</v>
       </c>
       <c r="J69" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K69" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L69" s="8" t="s">
         <v>655</v>
@@ -9465,10 +9471,10 @@
         <v>398</v>
       </c>
       <c r="J70" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K70" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L70" s="8" t="s">
         <v>645</v>
@@ -9531,10 +9537,10 @@
         <v>400</v>
       </c>
       <c r="J71" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K71" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L71" s="8" t="s">
         <v>135</v>
@@ -9601,10 +9607,10 @@
         <v>400</v>
       </c>
       <c r="J72" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K72" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L72" s="8" t="s">
         <v>310</v>
@@ -9671,10 +9677,10 @@
         <v>398</v>
       </c>
       <c r="J73" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K73" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L73" s="8" t="s">
         <v>68</v>
@@ -9735,10 +9741,10 @@
         <v>398</v>
       </c>
       <c r="J74" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K74" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L74" s="8" t="s">
         <v>673</v>
@@ -9799,10 +9805,10 @@
         <v>398</v>
       </c>
       <c r="J75" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K75" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L75" s="8" t="s">
         <v>444</v>
@@ -9865,10 +9871,10 @@
         <v>398</v>
       </c>
       <c r="J76" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K76" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L76" s="8" t="s">
         <v>187</v>
@@ -9931,10 +9937,10 @@
         <v>400</v>
       </c>
       <c r="J77" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K77" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L77" s="8" t="s">
         <v>497</v>
@@ -10001,10 +10007,10 @@
         <v>721</v>
       </c>
       <c r="J78" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K78" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L78" s="8" t="s">
         <v>69</v>
@@ -10067,10 +10073,10 @@
         <v>724</v>
       </c>
       <c r="J79" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K79" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L79" s="8" t="s">
         <v>69</v>
@@ -10133,10 +10139,10 @@
         <v>404</v>
       </c>
       <c r="J80" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K80" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L80" s="8" t="s">
         <v>69</v>
@@ -10199,10 +10205,10 @@
         <v>398</v>
       </c>
       <c r="J81" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K81" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L81" s="8" t="s">
         <v>69</v>
@@ -10265,10 +10271,10 @@
         <v>398</v>
       </c>
       <c r="J82" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K82" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L82" s="8" t="s">
         <v>69</v>
@@ -10331,10 +10337,10 @@
         <v>398</v>
       </c>
       <c r="J83" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K83" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L83" s="8" t="s">
         <v>69</v>
@@ -10397,10 +10403,10 @@
         <v>540</v>
       </c>
       <c r="J84" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K84" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L84" s="8" t="s">
         <v>736</v>
@@ -10463,10 +10469,10 @@
         <v>540</v>
       </c>
       <c r="J85" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K85" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L85" s="8" t="s">
         <v>738</v>
@@ -10529,10 +10535,10 @@
         <v>746</v>
       </c>
       <c r="J86" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K86" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L86" s="8" t="s">
         <v>68</v>
@@ -10593,10 +10599,10 @@
         <v>746</v>
       </c>
       <c r="J87" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K87" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L87" s="8"/>
       <c r="M87" s="8" t="s">
@@ -10657,10 +10663,10 @@
         <v>398</v>
       </c>
       <c r="J88" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K88" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L88" s="8" t="s">
         <v>69</v>
@@ -10723,10 +10729,10 @@
         <v>398</v>
       </c>
       <c r="J89" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K89" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L89" s="8" t="s">
         <v>69</v>
@@ -10789,10 +10795,10 @@
         <v>400</v>
       </c>
       <c r="J90" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K90" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L90" s="8" t="s">
         <v>69</v>
@@ -10855,10 +10861,10 @@
         <v>598</v>
       </c>
       <c r="J91" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K91" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L91" s="8" t="s">
         <v>69</v>
@@ -10921,10 +10927,10 @@
         <v>400</v>
       </c>
       <c r="J92" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K92" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L92" s="8" t="s">
         <v>69</v>
@@ -10987,10 +10993,10 @@
         <v>598</v>
       </c>
       <c r="J93" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K93" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L93" s="8" t="s">
         <v>69</v>
@@ -11053,10 +11059,10 @@
         <v>398</v>
       </c>
       <c r="J94" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K94" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L94" s="8" t="s">
         <v>69</v>
@@ -11119,10 +11125,10 @@
         <v>762</v>
       </c>
       <c r="J95" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K95" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L95" s="8" t="s">
         <v>69</v>
@@ -11185,10 +11191,10 @@
         <v>398</v>
       </c>
       <c r="J96" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K96" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L96" s="8" t="s">
         <v>69</v>
@@ -11251,10 +11257,10 @@
         <v>398</v>
       </c>
       <c r="J97" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K97" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L97" s="8" t="s">
         <v>69</v>
@@ -11317,10 +11323,10 @@
         <v>398</v>
       </c>
       <c r="J98" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K98" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L98" s="8" t="s">
         <v>69</v>
@@ -11383,10 +11389,10 @@
         <v>400</v>
       </c>
       <c r="J99" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K99" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L99" s="8" t="s">
         <v>69</v>
@@ -11449,10 +11455,10 @@
         <v>398</v>
       </c>
       <c r="J100" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K100" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L100" s="8" t="s">
         <v>69</v>
@@ -11515,10 +11521,10 @@
         <v>398</v>
       </c>
       <c r="J101" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K101" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L101" s="8" t="s">
         <v>69</v>
@@ -11581,10 +11587,10 @@
         <v>398</v>
       </c>
       <c r="J102" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K102" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L102" s="8" t="s">
         <v>69</v>
@@ -11647,10 +11653,10 @@
         <v>398</v>
       </c>
       <c r="J103" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K103" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L103" s="8" t="s">
         <v>69</v>
@@ -11713,10 +11719,10 @@
         <v>398</v>
       </c>
       <c r="J104" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K104" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L104" s="8" t="s">
         <v>69</v>
@@ -11779,10 +11785,10 @@
         <v>400</v>
       </c>
       <c r="J105" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K105" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L105" s="8" t="s">
         <v>69</v>
@@ -11845,10 +11851,10 @@
         <v>398</v>
       </c>
       <c r="J106" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K106" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L106" s="8" t="s">
         <v>69</v>
@@ -11911,10 +11917,10 @@
         <v>398</v>
       </c>
       <c r="J107" s="60" t="s">
-        <v>409</v>
+        <v>1184</v>
       </c>
       <c r="K107" s="60" t="s">
-        <v>410</v>
+        <v>1185</v>
       </c>
       <c r="L107" s="8" t="s">
         <v>69</v>
@@ -11976,11 +11982,11 @@
       <c r="I108" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="J108" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K108" s="27" t="s">
-        <v>410</v>
+      <c r="J108" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K108" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L108" s="27" t="s">
         <v>63</v>
@@ -12044,11 +12050,11 @@
       <c r="I109" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="J109" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K109" s="27" t="s">
-        <v>410</v>
+      <c r="J109" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K109" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L109" s="27" t="s">
         <v>64</v>
@@ -12112,11 +12118,11 @@
       <c r="I110" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="J110" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K110" s="27" t="s">
-        <v>410</v>
+      <c r="J110" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K110" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L110" s="27" t="s">
         <v>135</v>
@@ -12180,11 +12186,11 @@
       <c r="I111" s="27" t="s">
         <v>405</v>
       </c>
-      <c r="J111" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K111" s="27" t="s">
-        <v>410</v>
+      <c r="J111" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K111" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L111" s="27" t="s">
         <v>371</v>
@@ -12254,11 +12260,11 @@
       <c r="I112" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="J112" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K112" s="27" t="s">
-        <v>410</v>
+      <c r="J112" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K112" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L112" s="27" t="s">
         <v>142</v>
@@ -12322,11 +12328,11 @@
       <c r="I113" s="27" t="s">
         <v>402</v>
       </c>
-      <c r="J113" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K113" s="27" t="s">
-        <v>410</v>
+      <c r="J113" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K113" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L113" s="27" t="s">
         <v>310</v>
@@ -12396,11 +12402,11 @@
       <c r="I114" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="J114" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K114" s="27" t="s">
-        <v>410</v>
+      <c r="J114" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K114" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L114" s="27" t="s">
         <v>293</v>
@@ -12473,11 +12479,11 @@
       <c r="I115" s="27" t="s">
         <v>405</v>
       </c>
-      <c r="J115" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K115" s="27" t="s">
-        <v>410</v>
+      <c r="J115" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K115" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L115" s="27" t="s">
         <v>315</v>
@@ -12550,11 +12556,11 @@
       <c r="I116" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="J116" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K116" s="27" t="s">
-        <v>410</v>
+      <c r="J116" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K116" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L116" s="27" t="s">
         <v>258</v>
@@ -12618,11 +12624,11 @@
       <c r="I117" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="J117" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K117" s="27" t="s">
-        <v>410</v>
+      <c r="J117" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K117" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L117" s="27" t="s">
         <v>259</v>
@@ -12686,11 +12692,11 @@
       <c r="I118" s="27" t="s">
         <v>402</v>
       </c>
-      <c r="J118" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K118" s="27" t="s">
-        <v>410</v>
+      <c r="J118" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K118" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L118" s="27" t="s">
         <v>252</v>
@@ -12760,11 +12766,11 @@
       <c r="H119" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J119" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K119" s="27" t="s">
-        <v>410</v>
+      <c r="J119" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K119" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L119" s="27" t="s">
         <v>444</v>
@@ -12816,11 +12822,11 @@
       <c r="H120" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J120" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K120" s="27" t="s">
-        <v>410</v>
+      <c r="J120" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K120" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L120" s="27" t="s">
         <v>802</v>
@@ -12872,11 +12878,11 @@
       <c r="H121" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J121" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K121" s="27" t="s">
-        <v>410</v>
+      <c r="J121" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K121" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L121" s="71" t="s">
         <v>444</v>
@@ -12928,11 +12934,11 @@
       <c r="H122" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J122" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K122" s="27" t="s">
-        <v>410</v>
+      <c r="J122" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K122" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L122" s="71" t="s">
         <v>802</v>
@@ -12984,11 +12990,11 @@
       <c r="H123" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J123" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K123" s="27" t="s">
-        <v>410</v>
+      <c r="J123" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K123" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L123" s="71" t="s">
         <v>444</v>
@@ -13040,11 +13046,11 @@
       <c r="H124" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J124" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K124" s="27" t="s">
-        <v>410</v>
+      <c r="J124" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K124" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L124" s="71" t="s">
         <v>444</v>
@@ -13096,11 +13102,11 @@
       <c r="H125" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J125" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K125" s="27" t="s">
-        <v>410</v>
+      <c r="J125" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K125" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L125" s="27" t="s">
         <v>444</v>
@@ -13152,11 +13158,11 @@
       <c r="H126" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J126" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K126" s="27" t="s">
-        <v>410</v>
+      <c r="J126" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K126" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L126" s="27" t="s">
         <v>802</v>
@@ -13208,11 +13214,11 @@
       <c r="H127" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J127" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K127" s="27" t="s">
-        <v>410</v>
+      <c r="J127" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K127" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L127" s="71" t="s">
         <v>444</v>
@@ -13264,11 +13270,11 @@
       <c r="H128" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J128" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K128" s="27" t="s">
-        <v>410</v>
+      <c r="J128" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K128" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L128" s="71" t="s">
         <v>444</v>
@@ -13320,11 +13326,11 @@
       <c r="H129" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J129" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K129" s="27" t="s">
-        <v>410</v>
+      <c r="J129" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K129" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L129" s="27" t="s">
         <v>444</v>
@@ -13376,11 +13382,11 @@
       <c r="H130" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J130" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K130" s="27" t="s">
-        <v>410</v>
+      <c r="J130" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K130" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L130" s="27" t="s">
         <v>802</v>
@@ -13432,11 +13438,11 @@
       <c r="H131" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J131" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K131" s="27" t="s">
-        <v>410</v>
+      <c r="J131" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K131" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L131" s="69" t="s">
         <v>825</v>
@@ -13488,11 +13494,11 @@
       <c r="H132" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J132" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K132" s="27" t="s">
-        <v>410</v>
+      <c r="J132" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K132" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L132" s="69" t="s">
         <v>259</v>
@@ -13544,11 +13550,11 @@
       <c r="H133" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J133" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K133" s="27" t="s">
-        <v>410</v>
+      <c r="J133" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K133" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L133" s="71" t="s">
         <v>831</v>
@@ -13601,11 +13607,11 @@
       <c r="H134" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J134" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K134" s="27" t="s">
-        <v>410</v>
+      <c r="J134" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K134" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L134" s="27" t="s">
         <v>832</v>
@@ -13657,11 +13663,11 @@
       <c r="H135" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J135" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K135" s="27" t="s">
-        <v>410</v>
+      <c r="J135" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K135" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L135" s="27" t="s">
         <v>837</v>
@@ -13719,11 +13725,11 @@
       <c r="H136" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J136" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K136" s="27" t="s">
-        <v>410</v>
+      <c r="J136" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K136" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L136" s="27" t="s">
         <v>259</v>
@@ -13775,11 +13781,11 @@
       <c r="H137" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J137" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K137" s="27" t="s">
-        <v>410</v>
+      <c r="J137" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K137" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L137" s="34" t="s">
         <v>842</v>
@@ -13837,11 +13843,11 @@
       <c r="H138" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J138" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K138" s="27" t="s">
-        <v>410</v>
+      <c r="J138" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K138" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L138" s="74" t="s">
         <v>196</v>
@@ -13896,11 +13902,11 @@
       <c r="H139" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J139" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K139" s="27" t="s">
-        <v>410</v>
+      <c r="J139" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K139" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L139" s="27" t="s">
         <v>850</v>
@@ -13958,11 +13964,11 @@
       <c r="H140" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J140" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K140" s="27" t="s">
-        <v>410</v>
+      <c r="J140" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K140" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L140" s="27" t="s">
         <v>854</v>
@@ -14016,11 +14022,11 @@
       <c r="H141" s="76" t="s">
         <v>1182</v>
       </c>
-      <c r="J141" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="K141" s="27" t="s">
-        <v>410</v>
+      <c r="J141" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K141" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L141" s="27" t="s">
         <v>859</v>
@@ -14081,11 +14087,11 @@
       <c r="I142" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="J142" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K142" s="16" t="s">
-        <v>410</v>
+      <c r="J142" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K142" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L142" s="10" t="s">
         <v>938</v>
@@ -14156,11 +14162,11 @@
       <c r="I143" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J143" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K143" s="16" t="s">
-        <v>410</v>
+      <c r="J143" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K143" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L143" s="8" t="s">
         <v>444</v>
@@ -14227,11 +14233,11 @@
       <c r="I144" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J144" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K144" s="16" t="s">
-        <v>410</v>
+      <c r="J144" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K144" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L144" s="8" t="s">
         <v>943</v>
@@ -14298,11 +14304,11 @@
       <c r="I145" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J145" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K145" s="16" t="s">
-        <v>410</v>
+      <c r="J145" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K145" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L145" s="8" t="s">
         <v>263</v>
@@ -14369,11 +14375,11 @@
       <c r="I146" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J146" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K146" s="16" t="s">
-        <v>410</v>
+      <c r="J146" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K146" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L146" s="10" t="s">
         <v>264</v>
@@ -14440,11 +14446,11 @@
       <c r="I147" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="J147" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K147" s="16" t="s">
-        <v>410</v>
+      <c r="J147" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K147" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L147" s="8" t="s">
         <v>324</v>
@@ -14515,11 +14521,11 @@
       <c r="I148" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J148" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K148" s="16" t="s">
-        <v>410</v>
+      <c r="J148" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K148" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L148" s="8" t="s">
         <v>948</v>
@@ -14590,11 +14596,11 @@
       <c r="I149" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="J149" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K149" s="16" t="s">
-        <v>410</v>
+      <c r="J149" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K149" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L149" s="8" t="s">
         <v>953</v>
@@ -14668,11 +14674,11 @@
       <c r="I150" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="J150" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K150" s="16" t="s">
-        <v>410</v>
+      <c r="J150" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K150" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L150" s="8" t="s">
         <v>957</v>
@@ -14739,11 +14745,11 @@
       <c r="I151" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="J151" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K151" s="16" t="s">
-        <v>410</v>
+      <c r="J151" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K151" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L151" s="10" t="s">
         <v>961</v>
@@ -14810,11 +14816,11 @@
       <c r="I152" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="J152" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K152" s="16" t="s">
-        <v>410</v>
+      <c r="J152" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K152" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L152" s="8" t="s">
         <v>259</v>
@@ -14881,11 +14887,11 @@
       <c r="I153" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="J153" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K153" s="16" t="s">
-        <v>410</v>
+      <c r="J153" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K153" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L153" s="8" t="s">
         <v>324</v>
@@ -14956,11 +14962,11 @@
       <c r="I154" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J154" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K154" s="16" t="s">
-        <v>410</v>
+      <c r="J154" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K154" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L154" s="8" t="s">
         <v>126</v>
@@ -15027,11 +15033,11 @@
       <c r="I155" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J155" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K155" s="16" t="s">
-        <v>410</v>
+      <c r="J155" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K155" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L155" s="8" t="s">
         <v>132</v>
@@ -15098,11 +15104,11 @@
       <c r="I156" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="J156" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K156" s="16" t="s">
-        <v>410</v>
+      <c r="J156" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K156" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L156" s="8" t="s">
         <v>259</v>
@@ -15172,11 +15178,11 @@
       <c r="I157" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="J157" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K157" s="16" t="s">
-        <v>410</v>
+      <c r="J157" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K157" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L157" s="10" t="s">
         <v>968</v>
@@ -15250,11 +15256,11 @@
       <c r="I158" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="J158" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K158" s="16" t="s">
-        <v>410</v>
+      <c r="J158" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K158" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L158" s="8" t="s">
         <v>69</v>
@@ -15321,11 +15327,11 @@
       <c r="I159" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="J159" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K159" s="16" t="s">
-        <v>410</v>
+      <c r="J159" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K159" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L159" s="10" t="s">
         <v>70</v>
@@ -15392,11 +15398,11 @@
       <c r="I160" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="J160" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K160" s="16" t="s">
-        <v>410</v>
+      <c r="J160" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K160" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L160" t="s">
         <v>66</v>
@@ -15463,11 +15469,11 @@
       <c r="I161" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="J161" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K161" s="16" t="s">
-        <v>410</v>
+      <c r="J161" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K161" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L161" s="10" t="s">
         <v>70</v>
@@ -15534,11 +15540,11 @@
       <c r="I162" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="J162" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K162" s="16" t="s">
-        <v>410</v>
+      <c r="J162" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K162" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L162" s="8" t="s">
         <v>68</v>
@@ -15605,11 +15611,11 @@
       <c r="I163" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="J163" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K163" s="16" t="s">
-        <v>410</v>
+      <c r="J163" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K163" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L163" s="10" t="s">
         <v>978</v>
@@ -15676,11 +15682,11 @@
       <c r="I164" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="J164" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K164" s="16" t="s">
-        <v>410</v>
+      <c r="J164" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K164" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L164" s="16" t="s">
         <v>1045</v>
@@ -15735,11 +15741,11 @@
       <c r="I165" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="J165" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K165" s="16" t="s">
-        <v>410</v>
+      <c r="J165" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K165" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L165" s="16" t="s">
         <v>118</v>
@@ -15794,11 +15800,11 @@
       <c r="I166" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="J166" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K166" s="16" t="s">
-        <v>410</v>
+      <c r="J166" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K166" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L166" s="16" t="s">
         <v>304</v>
@@ -15853,11 +15859,11 @@
       <c r="I167" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="J167" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K167" s="16" t="s">
-        <v>410</v>
+      <c r="J167" s="60" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K167" s="60" t="s">
+        <v>1185</v>
       </c>
       <c r="L167" s="16" t="s">
         <v>306</v>
@@ -16828,7 +16834,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="184" spans="1:28" ht="15.75" thickBot="1">
+    <row r="184" spans="1:28" ht="30.75" thickBot="1">
       <c r="A184" s="7">
         <v>17931</v>
       </c>
@@ -17342,24 +17348,24 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="82"/>
+      <c r="B8" s="83"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
       <c r="I9" t="s">
         <v>44</v>
       </c>
@@ -17368,15 +17374,15 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
       <c r="I10" t="s">
         <v>46</v>
       </c>
@@ -17385,15 +17391,15 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
       <c r="I11" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Update the Report generation file path
</commit_message>
<xml_diff>
--- a/PartnerMasterConfiguration.xlsx
+++ b/PartnerMasterConfiguration.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D5EBFE-7E79-44C0-BD0F-2C1C49B71ADB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353B77CD-DBDB-40EA-BBA0-B59AE143D716}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7597" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7597" uniqueCount="1179">
   <si>
     <t>Partner ID</t>
   </si>
@@ -3653,6 +3653,12 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>D:\ArloVerisure\Source\&lt;Partner ID&gt;\&lt;POS_Inventory_Flag&gt;\DDMMYY\Original\&lt;original_file_name&gt;</t>
+  </si>
+  <si>
+    <t>D:\ArloVerisure\Transformed\&lt;Partner ID&gt;\&lt;POS_Inventory_Flag&gt;\DDMMYY\&lt;renamed_file&gt;</t>
   </si>
 </sst>
 </file>
@@ -4681,10 +4687,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB186"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2:K165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4833,10 +4839,10 @@
         <v>393</v>
       </c>
       <c r="J2" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K2" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L2" s="60" t="s">
         <v>64</v>
@@ -4907,10 +4913,10 @@
         <v>393</v>
       </c>
       <c r="J3" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K3" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L3" s="60" t="s">
         <v>66</v>
@@ -4981,10 +4987,10 @@
         <v>396</v>
       </c>
       <c r="J4" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K4" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L4" s="60" t="s">
         <v>119</v>
@@ -5055,10 +5061,10 @@
         <v>396</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K5" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L5" s="60" t="s">
         <v>121</v>
@@ -5129,10 +5135,10 @@
         <v>401</v>
       </c>
       <c r="J6" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K6" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L6" s="60" t="s">
         <v>198</v>
@@ -5203,10 +5209,10 @@
         <v>401</v>
       </c>
       <c r="J7" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K7" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L7" s="60" t="s">
         <v>210</v>
@@ -5277,10 +5283,10 @@
         <v>401</v>
       </c>
       <c r="J8" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K8" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L8" s="60" t="s">
         <v>280</v>
@@ -5357,10 +5363,10 @@
         <v>398</v>
       </c>
       <c r="J9" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K9" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L9" s="60" t="s">
         <v>296</v>
@@ -5435,10 +5441,10 @@
         <v>395</v>
       </c>
       <c r="J10" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K10" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L10" s="60" t="s">
         <v>320</v>
@@ -5511,10 +5517,10 @@
       </c>
       <c r="I11" s="60"/>
       <c r="J11" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K11" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L11" s="60" t="s">
         <v>411</v>
@@ -5579,10 +5585,10 @@
       </c>
       <c r="I12" s="60"/>
       <c r="J12" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K12" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L12" s="60" t="s">
         <v>340</v>
@@ -5645,10 +5651,10 @@
         <v>394</v>
       </c>
       <c r="J13" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K13" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>430</v>
@@ -5713,10 +5719,10 @@
         <v>394</v>
       </c>
       <c r="J14" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K14" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>431</v>
@@ -5781,10 +5787,10 @@
         <v>400</v>
       </c>
       <c r="J15" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K15" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>440</v>
@@ -5849,10 +5855,10 @@
         <v>400</v>
       </c>
       <c r="J16" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K16" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>441</v>
@@ -5917,10 +5923,10 @@
         <v>396</v>
       </c>
       <c r="J17" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K17" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>440</v>
@@ -5979,10 +5985,10 @@
         <v>396</v>
       </c>
       <c r="J18" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K18" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>441</v>
@@ -6041,10 +6047,10 @@
         <v>394</v>
       </c>
       <c r="J19" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K19" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>459</v>
@@ -6107,10 +6113,10 @@
         <v>394</v>
       </c>
       <c r="J20" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K20" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>109</v>
@@ -6170,10 +6176,10 @@
         <v>394</v>
       </c>
       <c r="J21" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K21" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>477</v>
@@ -6229,10 +6235,10 @@
         <v>400</v>
       </c>
       <c r="J22" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K22" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>340</v>
@@ -6292,10 +6298,10 @@
         <v>400</v>
       </c>
       <c r="J23" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K23" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>222</v>
@@ -6355,10 +6361,10 @@
         <v>400</v>
       </c>
       <c r="J24" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K24" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L24" s="60" t="s">
         <v>136</v>
@@ -6433,10 +6439,10 @@
         <v>396</v>
       </c>
       <c r="J25" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K25" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L25" s="60" t="s">
         <v>219</v>
@@ -6511,10 +6517,10 @@
         <v>396</v>
       </c>
       <c r="J26" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K26" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>499</v>
@@ -6579,10 +6585,10 @@
         <v>396</v>
       </c>
       <c r="J27" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K27" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L27" s="60" t="s">
         <v>67</v>
@@ -6653,10 +6659,10 @@
         <v>396</v>
       </c>
       <c r="J28" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K28" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L28" s="60" t="s">
         <v>217</v>
@@ -6727,10 +6733,10 @@
         <v>400</v>
       </c>
       <c r="J29" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K29" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>508</v>
@@ -6792,10 +6798,10 @@
         <v>400</v>
       </c>
       <c r="J30" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K30" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>517</v>
@@ -6858,10 +6864,10 @@
         <v>400</v>
       </c>
       <c r="J31" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K31" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>521</v>
@@ -6924,10 +6930,10 @@
         <v>400</v>
       </c>
       <c r="J32" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K32" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>187</v>
@@ -6988,10 +6994,10 @@
         <v>400</v>
       </c>
       <c r="J33" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K33" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>526</v>
@@ -7047,10 +7053,10 @@
         <v>397</v>
       </c>
       <c r="J34" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K34" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>124</v>
@@ -7111,10 +7117,10 @@
         <v>399</v>
       </c>
       <c r="J35" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K35" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>133</v>
@@ -7175,10 +7181,10 @@
         <v>399</v>
       </c>
       <c r="J36" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K36" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L36" s="8" t="s">
         <v>134</v>
@@ -7239,10 +7245,10 @@
         <v>536</v>
       </c>
       <c r="J37" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K37" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L37" s="8" t="s">
         <v>537</v>
@@ -7305,10 +7311,10 @@
         <v>536</v>
       </c>
       <c r="J38" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K38" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L38" s="8" t="s">
         <v>538</v>
@@ -7371,10 +7377,10 @@
         <v>394</v>
       </c>
       <c r="J39" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K39" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>547</v>
@@ -7437,10 +7443,10 @@
         <v>394</v>
       </c>
       <c r="J40" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K40" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>548</v>
@@ -7503,10 +7509,10 @@
         <v>396</v>
       </c>
       <c r="J41" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K41" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>136</v>
@@ -7571,10 +7577,10 @@
         <v>400</v>
       </c>
       <c r="J42" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K42" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>556</v>
@@ -7637,10 +7643,10 @@
         <v>400</v>
       </c>
       <c r="J43" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K43" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>557</v>
@@ -7703,10 +7709,10 @@
         <v>396</v>
       </c>
       <c r="J44" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K44" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>563</v>
@@ -7771,10 +7777,10 @@
         <v>394</v>
       </c>
       <c r="J45" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K45" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L45" s="8" t="s">
         <v>567</v>
@@ -7839,10 +7845,10 @@
         <v>394</v>
       </c>
       <c r="J46" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K46" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L46" s="8" t="s">
         <v>568</v>
@@ -7907,10 +7913,10 @@
         <v>400</v>
       </c>
       <c r="J47" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K47" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L47" s="8" t="s">
         <v>563</v>
@@ -7971,10 +7977,10 @@
         <v>394</v>
       </c>
       <c r="J48" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K48" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L48" s="8" t="s">
         <v>292</v>
@@ -8035,10 +8041,10 @@
         <v>396</v>
       </c>
       <c r="J49" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K49" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>585</v>
@@ -8103,10 +8109,10 @@
         <v>594</v>
       </c>
       <c r="J50" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K50" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L50" s="8" t="s">
         <v>595</v>
@@ -8171,10 +8177,10 @@
         <v>396</v>
       </c>
       <c r="J51" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K51" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L51" s="8" t="s">
         <v>105</v>
@@ -8232,10 +8238,10 @@
         <v>396</v>
       </c>
       <c r="J52" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K52" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L52" s="8" t="s">
         <v>16</v>
@@ -8293,10 +8299,10 @@
         <v>594</v>
       </c>
       <c r="J53" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K53" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L53" s="8" t="s">
         <v>105</v>
@@ -8359,10 +8365,10 @@
         <v>594</v>
       </c>
       <c r="J54" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K54" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L54" s="8" t="s">
         <v>16</v>
@@ -8425,10 +8431,10 @@
         <v>394</v>
       </c>
       <c r="J55" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K55" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>105</v>
@@ -8491,10 +8497,10 @@
         <v>394</v>
       </c>
       <c r="J56" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K56" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L56" s="8" t="s">
         <v>16</v>
@@ -8557,10 +8563,10 @@
         <v>394</v>
       </c>
       <c r="J57" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K57" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L57" s="8" t="s">
         <v>440</v>
@@ -8623,10 +8629,10 @@
         <v>394</v>
       </c>
       <c r="J58" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K58" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L58" s="8" t="s">
         <v>610</v>
@@ -8689,10 +8695,10 @@
         <v>394</v>
       </c>
       <c r="J59" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K59" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L59" s="8" t="s">
         <v>614</v>
@@ -8755,10 +8761,10 @@
         <v>394</v>
       </c>
       <c r="J60" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K60" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L60" s="8" t="s">
         <v>616</v>
@@ -8821,10 +8827,10 @@
         <v>394</v>
       </c>
       <c r="J61" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K61" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L61" s="8" t="s">
         <v>620</v>
@@ -8887,10 +8893,10 @@
         <v>394</v>
       </c>
       <c r="J62" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K62" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L62" s="8" t="s">
         <v>622</v>
@@ -8953,10 +8959,10 @@
         <v>394</v>
       </c>
       <c r="J63" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K63" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L63" s="8" t="s">
         <v>624</v>
@@ -9019,10 +9025,10 @@
         <v>396</v>
       </c>
       <c r="J64" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K64" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L64" s="8" t="s">
         <v>634</v>
@@ -9087,10 +9093,10 @@
         <v>394</v>
       </c>
       <c r="J65" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K65" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L65" s="8" t="s">
         <v>641</v>
@@ -9153,10 +9159,10 @@
         <v>649</v>
       </c>
       <c r="J66" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K66" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L66" s="8" t="s">
         <v>67</v>
@@ -9219,10 +9225,10 @@
         <v>649</v>
       </c>
       <c r="J67" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K67" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L67" s="8" t="s">
         <v>651</v>
@@ -9285,10 +9291,10 @@
         <v>394</v>
       </c>
       <c r="J68" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K68" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L68" s="8" t="s">
         <v>641</v>
@@ -9351,10 +9357,10 @@
         <v>396</v>
       </c>
       <c r="J69" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K69" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L69" s="8" t="s">
         <v>133</v>
@@ -9421,10 +9427,10 @@
         <v>396</v>
       </c>
       <c r="J70" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K70" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L70" s="8" t="s">
         <v>306</v>
@@ -9491,10 +9497,10 @@
         <v>394</v>
       </c>
       <c r="J71" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K71" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L71" s="8" t="s">
         <v>67</v>
@@ -9555,10 +9561,10 @@
         <v>394</v>
       </c>
       <c r="J72" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K72" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L72" s="8" t="s">
         <v>669</v>
@@ -9619,10 +9625,10 @@
         <v>394</v>
       </c>
       <c r="J73" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K73" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L73" s="8" t="s">
         <v>440</v>
@@ -9685,10 +9691,10 @@
         <v>394</v>
       </c>
       <c r="J74" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K74" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L74" s="8" t="s">
         <v>183</v>
@@ -9751,10 +9757,10 @@
         <v>396</v>
       </c>
       <c r="J75" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K75" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L75" s="8" t="s">
         <v>493</v>
@@ -9821,10 +9827,10 @@
         <v>717</v>
       </c>
       <c r="J76" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K76" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L76" s="8" t="s">
         <v>68</v>
@@ -9887,10 +9893,10 @@
         <v>720</v>
       </c>
       <c r="J77" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K77" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L77" s="8" t="s">
         <v>68</v>
@@ -9953,10 +9959,10 @@
         <v>400</v>
       </c>
       <c r="J78" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K78" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L78" s="8" t="s">
         <v>68</v>
@@ -10019,10 +10025,10 @@
         <v>394</v>
       </c>
       <c r="J79" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K79" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L79" s="8" t="s">
         <v>68</v>
@@ -10085,10 +10091,10 @@
         <v>394</v>
       </c>
       <c r="J80" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K80" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L80" s="8" t="s">
         <v>68</v>
@@ -10151,10 +10157,10 @@
         <v>394</v>
       </c>
       <c r="J81" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K81" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L81" s="8" t="s">
         <v>68</v>
@@ -10217,10 +10223,10 @@
         <v>536</v>
       </c>
       <c r="J82" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K82" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L82" s="8" t="s">
         <v>732</v>
@@ -10283,10 +10289,10 @@
         <v>536</v>
       </c>
       <c r="J83" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K83" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L83" s="8" t="s">
         <v>734</v>
@@ -10349,10 +10355,10 @@
         <v>742</v>
       </c>
       <c r="J84" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K84" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L84" s="8" t="s">
         <v>67</v>
@@ -10413,10 +10419,10 @@
         <v>742</v>
       </c>
       <c r="J85" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K85" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L85" s="8"/>
       <c r="M85" s="8" t="s">
@@ -10477,10 +10483,10 @@
         <v>394</v>
       </c>
       <c r="J86" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K86" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L86" s="8" t="s">
         <v>68</v>
@@ -10543,10 +10549,10 @@
         <v>394</v>
       </c>
       <c r="J87" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K87" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L87" s="8" t="s">
         <v>68</v>
@@ -10609,10 +10615,10 @@
         <v>396</v>
       </c>
       <c r="J88" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K88" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L88" s="8" t="s">
         <v>68</v>
@@ -10675,10 +10681,10 @@
         <v>594</v>
       </c>
       <c r="J89" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K89" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L89" s="8" t="s">
         <v>68</v>
@@ -10741,10 +10747,10 @@
         <v>396</v>
       </c>
       <c r="J90" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K90" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L90" s="8" t="s">
         <v>68</v>
@@ -10807,10 +10813,10 @@
         <v>594</v>
       </c>
       <c r="J91" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K91" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L91" s="8" t="s">
         <v>68</v>
@@ -10873,10 +10879,10 @@
         <v>394</v>
       </c>
       <c r="J92" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K92" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L92" s="8" t="s">
         <v>68</v>
@@ -10939,10 +10945,10 @@
         <v>758</v>
       </c>
       <c r="J93" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K93" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L93" s="8" t="s">
         <v>68</v>
@@ -11005,10 +11011,10 @@
         <v>394</v>
       </c>
       <c r="J94" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K94" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L94" s="8" t="s">
         <v>68</v>
@@ -11071,10 +11077,10 @@
         <v>394</v>
       </c>
       <c r="J95" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K95" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L95" s="8" t="s">
         <v>68</v>
@@ -11137,10 +11143,10 @@
         <v>394</v>
       </c>
       <c r="J96" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K96" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L96" s="8" t="s">
         <v>68</v>
@@ -11203,10 +11209,10 @@
         <v>396</v>
       </c>
       <c r="J97" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K97" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L97" s="8" t="s">
         <v>68</v>
@@ -11269,10 +11275,10 @@
         <v>394</v>
       </c>
       <c r="J98" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K98" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L98" s="8" t="s">
         <v>68</v>
@@ -11335,10 +11341,10 @@
         <v>394</v>
       </c>
       <c r="J99" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K99" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L99" s="8" t="s">
         <v>68</v>
@@ -11401,10 +11407,10 @@
         <v>394</v>
       </c>
       <c r="J100" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K100" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L100" s="8" t="s">
         <v>68</v>
@@ -11467,10 +11473,10 @@
         <v>394</v>
       </c>
       <c r="J101" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K101" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L101" s="8" t="s">
         <v>68</v>
@@ -11533,10 +11539,10 @@
         <v>394</v>
       </c>
       <c r="J102" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K102" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L102" s="8" t="s">
         <v>68</v>
@@ -11599,10 +11605,10 @@
         <v>396</v>
       </c>
       <c r="J103" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K103" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L103" s="8" t="s">
         <v>68</v>
@@ -11665,10 +11671,10 @@
         <v>394</v>
       </c>
       <c r="J104" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K104" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L104" s="8" t="s">
         <v>68</v>
@@ -11731,10 +11737,10 @@
         <v>394</v>
       </c>
       <c r="J105" s="60" t="s">
-        <v>405</v>
+        <v>1177</v>
       </c>
       <c r="K105" s="60" t="s">
-        <v>406</v>
+        <v>1178</v>
       </c>
       <c r="L105" s="8" t="s">
         <v>68</v>
@@ -11796,11 +11802,11 @@
       <c r="I106" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="J106" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K106" s="27" t="s">
-        <v>406</v>
+      <c r="J106" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K106" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L106" s="27" t="s">
         <v>62</v>
@@ -11864,11 +11870,11 @@
       <c r="I107" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="J107" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K107" s="27" t="s">
-        <v>406</v>
+      <c r="J107" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K107" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L107" s="27" t="s">
         <v>63</v>
@@ -11932,11 +11938,11 @@
       <c r="I108" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="J108" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K108" s="27" t="s">
-        <v>406</v>
+      <c r="J108" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K108" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L108" s="27" t="s">
         <v>133</v>
@@ -12000,11 +12006,11 @@
       <c r="I109" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="J109" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K109" s="27" t="s">
-        <v>406</v>
+      <c r="J109" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K109" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L109" s="27" t="s">
         <v>367</v>
@@ -12074,11 +12080,11 @@
       <c r="I110" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="J110" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K110" s="27" t="s">
-        <v>406</v>
+      <c r="J110" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K110" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L110" s="27" t="s">
         <v>139</v>
@@ -12142,11 +12148,11 @@
       <c r="I111" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="J111" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K111" s="27" t="s">
-        <v>406</v>
+      <c r="J111" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K111" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L111" s="27" t="s">
         <v>306</v>
@@ -12216,11 +12222,11 @@
       <c r="I112" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="J112" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K112" s="27" t="s">
-        <v>406</v>
+      <c r="J112" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K112" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L112" s="27" t="s">
         <v>289</v>
@@ -12293,11 +12299,11 @@
       <c r="I113" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="J113" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K113" s="27" t="s">
-        <v>406</v>
+      <c r="J113" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K113" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L113" s="27" t="s">
         <v>311</v>
@@ -12370,11 +12376,11 @@
       <c r="I114" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="J114" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K114" s="27" t="s">
-        <v>406</v>
+      <c r="J114" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K114" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L114" s="27" t="s">
         <v>254</v>
@@ -12438,11 +12444,11 @@
       <c r="I115" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="J115" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K115" s="27" t="s">
-        <v>406</v>
+      <c r="J115" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K115" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L115" s="27" t="s">
         <v>255</v>
@@ -12506,11 +12512,11 @@
       <c r="I116" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="J116" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K116" s="27" t="s">
-        <v>406</v>
+      <c r="J116" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K116" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L116" s="27" t="s">
         <v>248</v>
@@ -12580,11 +12586,11 @@
       <c r="H117" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J117" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K117" s="27" t="s">
-        <v>406</v>
+      <c r="J117" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K117" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L117" s="27" t="s">
         <v>440</v>
@@ -12636,11 +12642,11 @@
       <c r="H118" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J118" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K118" s="27" t="s">
-        <v>406</v>
+      <c r="J118" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K118" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L118" s="27" t="s">
         <v>798</v>
@@ -12692,11 +12698,11 @@
       <c r="H119" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J119" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K119" s="27" t="s">
-        <v>406</v>
+      <c r="J119" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K119" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L119" s="71" t="s">
         <v>440</v>
@@ -12748,11 +12754,11 @@
       <c r="H120" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J120" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K120" s="27" t="s">
-        <v>406</v>
+      <c r="J120" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K120" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L120" s="71" t="s">
         <v>798</v>
@@ -12804,11 +12810,11 @@
       <c r="H121" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J121" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K121" s="27" t="s">
-        <v>406</v>
+      <c r="J121" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K121" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L121" s="71" t="s">
         <v>440</v>
@@ -12860,11 +12866,11 @@
       <c r="H122" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J122" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K122" s="27" t="s">
-        <v>406</v>
+      <c r="J122" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K122" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L122" s="71" t="s">
         <v>440</v>
@@ -12916,11 +12922,11 @@
       <c r="H123" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J123" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K123" s="27" t="s">
-        <v>406</v>
+      <c r="J123" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K123" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L123" s="27" t="s">
         <v>440</v>
@@ -12972,11 +12978,11 @@
       <c r="H124" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J124" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K124" s="27" t="s">
-        <v>406</v>
+      <c r="J124" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K124" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L124" s="27" t="s">
         <v>798</v>
@@ -13028,11 +13034,11 @@
       <c r="H125" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J125" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K125" s="27" t="s">
-        <v>406</v>
+      <c r="J125" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K125" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L125" s="71" t="s">
         <v>440</v>
@@ -13084,11 +13090,11 @@
       <c r="H126" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J126" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K126" s="27" t="s">
-        <v>406</v>
+      <c r="J126" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K126" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L126" s="71" t="s">
         <v>440</v>
@@ -13140,11 +13146,11 @@
       <c r="H127" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J127" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K127" s="27" t="s">
-        <v>406</v>
+      <c r="J127" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K127" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L127" s="27" t="s">
         <v>440</v>
@@ -13196,11 +13202,11 @@
       <c r="H128" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J128" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K128" s="27" t="s">
-        <v>406</v>
+      <c r="J128" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K128" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L128" s="27" t="s">
         <v>798</v>
@@ -13252,11 +13258,11 @@
       <c r="H129" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J129" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K129" s="27" t="s">
-        <v>406</v>
+      <c r="J129" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K129" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L129" s="69" t="s">
         <v>821</v>
@@ -13308,11 +13314,11 @@
       <c r="H130" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J130" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K130" s="27" t="s">
-        <v>406</v>
+      <c r="J130" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K130" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L130" s="69" t="s">
         <v>255</v>
@@ -13364,11 +13370,11 @@
       <c r="H131" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J131" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K131" s="27" t="s">
-        <v>406</v>
+      <c r="J131" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K131" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L131" s="71" t="s">
         <v>827</v>
@@ -13421,11 +13427,11 @@
       <c r="H132" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J132" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K132" s="27" t="s">
-        <v>406</v>
+      <c r="J132" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K132" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L132" s="27" t="s">
         <v>828</v>
@@ -13477,11 +13483,11 @@
       <c r="H133" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J133" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K133" s="27" t="s">
-        <v>406</v>
+      <c r="J133" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K133" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L133" s="27" t="s">
         <v>833</v>
@@ -13539,11 +13545,11 @@
       <c r="H134" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J134" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K134" s="27" t="s">
-        <v>406</v>
+      <c r="J134" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K134" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L134" s="27" t="s">
         <v>255</v>
@@ -13595,11 +13601,11 @@
       <c r="H135" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J135" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K135" s="27" t="s">
-        <v>406</v>
+      <c r="J135" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K135" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L135" s="34" t="s">
         <v>838</v>
@@ -13657,11 +13663,11 @@
       <c r="H136" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J136" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K136" s="27" t="s">
-        <v>406</v>
+      <c r="J136" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K136" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L136" s="74" t="s">
         <v>192</v>
@@ -13716,11 +13722,11 @@
       <c r="H137" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J137" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K137" s="27" t="s">
-        <v>406</v>
+      <c r="J137" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K137" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L137" s="27" t="s">
         <v>846</v>
@@ -13778,11 +13784,11 @@
       <c r="H138" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J138" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K138" s="27" t="s">
-        <v>406</v>
+      <c r="J138" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K138" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L138" s="27" t="s">
         <v>850</v>
@@ -13836,11 +13842,11 @@
       <c r="H139" s="76" t="s">
         <v>1172</v>
       </c>
-      <c r="J139" s="27" t="s">
-        <v>405</v>
-      </c>
-      <c r="K139" s="27" t="s">
-        <v>406</v>
+      <c r="J139" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K139" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L139" s="27" t="s">
         <v>855</v>
@@ -13901,11 +13907,11 @@
       <c r="I140" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="J140" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K140" s="16" t="s">
-        <v>406</v>
+      <c r="J140" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K140" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L140" s="10" t="s">
         <v>934</v>
@@ -13976,11 +13982,11 @@
       <c r="I141" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J141" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K141" s="16" t="s">
-        <v>406</v>
+      <c r="J141" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K141" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L141" s="8" t="s">
         <v>440</v>
@@ -14047,11 +14053,11 @@
       <c r="I142" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J142" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K142" s="16" t="s">
-        <v>406</v>
+      <c r="J142" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K142" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L142" s="8" t="s">
         <v>939</v>
@@ -14118,11 +14124,11 @@
       <c r="I143" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J143" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K143" s="16" t="s">
-        <v>406</v>
+      <c r="J143" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K143" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L143" s="8" t="s">
         <v>259</v>
@@ -14189,11 +14195,11 @@
       <c r="I144" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J144" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K144" s="16" t="s">
-        <v>406</v>
+      <c r="J144" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K144" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L144" s="10" t="s">
         <v>260</v>
@@ -14260,11 +14266,11 @@
       <c r="I145" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="J145" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K145" s="16" t="s">
-        <v>406</v>
+      <c r="J145" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K145" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L145" s="8" t="s">
         <v>320</v>
@@ -14335,11 +14341,11 @@
       <c r="I146" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J146" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K146" s="16" t="s">
-        <v>406</v>
+      <c r="J146" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K146" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L146" s="8" t="s">
         <v>944</v>
@@ -14410,11 +14416,11 @@
       <c r="I147" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="J147" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K147" s="16" t="s">
-        <v>406</v>
+      <c r="J147" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K147" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L147" s="8" t="s">
         <v>949</v>
@@ -14488,11 +14494,11 @@
       <c r="I148" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J148" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K148" s="16" t="s">
-        <v>406</v>
+      <c r="J148" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K148" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L148" s="8" t="s">
         <v>953</v>
@@ -14559,11 +14565,11 @@
       <c r="I149" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J149" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K149" s="16" t="s">
-        <v>406</v>
+      <c r="J149" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K149" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L149" s="10" t="s">
         <v>957</v>
@@ -14630,11 +14636,11 @@
       <c r="I150" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="J150" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K150" s="16" t="s">
-        <v>406</v>
+      <c r="J150" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K150" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L150" s="8" t="s">
         <v>255</v>
@@ -14701,11 +14707,11 @@
       <c r="I151" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="J151" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K151" s="16" t="s">
-        <v>406</v>
+      <c r="J151" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K151" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L151" s="8" t="s">
         <v>320</v>
@@ -14776,11 +14782,11 @@
       <c r="I152" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J152" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K152" s="16" t="s">
-        <v>406</v>
+      <c r="J152" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K152" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L152" s="8" t="s">
         <v>124</v>
@@ -14847,11 +14853,11 @@
       <c r="I153" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="J153" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K153" s="16" t="s">
-        <v>406</v>
+      <c r="J153" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K153" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L153" s="8" t="s">
         <v>130</v>
@@ -14918,11 +14924,11 @@
       <c r="I154" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="J154" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K154" s="16" t="s">
-        <v>406</v>
+      <c r="J154" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K154" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L154" s="8" t="s">
         <v>255</v>
@@ -14992,11 +14998,11 @@
       <c r="I155" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="J155" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K155" s="16" t="s">
-        <v>406</v>
+      <c r="J155" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K155" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L155" s="10" t="s">
         <v>964</v>
@@ -15070,11 +15076,11 @@
       <c r="I156" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="J156" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K156" s="16" t="s">
-        <v>406</v>
+      <c r="J156" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K156" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L156" s="8" t="s">
         <v>68</v>
@@ -15141,11 +15147,11 @@
       <c r="I157" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="J157" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K157" s="16" t="s">
-        <v>406</v>
+      <c r="J157" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K157" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L157" s="10" t="s">
         <v>69</v>
@@ -15212,11 +15218,11 @@
       <c r="I158" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="J158" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K158" s="16" t="s">
-        <v>406</v>
+      <c r="J158" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K158" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L158" t="s">
         <v>65</v>
@@ -15283,11 +15289,11 @@
       <c r="I159" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="J159" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K159" s="16" t="s">
-        <v>406</v>
+      <c r="J159" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K159" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L159" s="10" t="s">
         <v>69</v>
@@ -15354,11 +15360,11 @@
       <c r="I160" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="J160" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K160" s="16" t="s">
-        <v>406</v>
+      <c r="J160" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K160" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L160" s="8" t="s">
         <v>67</v>
@@ -15425,11 +15431,11 @@
       <c r="I161" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="J161" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K161" s="16" t="s">
-        <v>406</v>
+      <c r="J161" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K161" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L161" s="10" t="s">
         <v>974</v>
@@ -15496,11 +15502,11 @@
       <c r="I162" s="16" t="s">
         <v>395</v>
       </c>
-      <c r="J162" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K162" s="16" t="s">
-        <v>406</v>
+      <c r="J162" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K162" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L162" s="16" t="s">
         <v>1041</v>
@@ -15555,11 +15561,11 @@
       <c r="I163" s="16" t="s">
         <v>395</v>
       </c>
-      <c r="J163" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K163" s="16" t="s">
-        <v>406</v>
+      <c r="J163" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K163" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L163" s="16" t="s">
         <v>116</v>
@@ -15614,11 +15620,11 @@
       <c r="I164" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="J164" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K164" s="16" t="s">
-        <v>406</v>
+      <c r="J164" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K164" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L164" s="16" t="s">
         <v>300</v>
@@ -15673,11 +15679,11 @@
       <c r="I165" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="J165" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="K165" s="16" t="s">
-        <v>406</v>
+      <c r="J165" s="60" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K165" s="60" t="s">
+        <v>1178</v>
       </c>
       <c r="L165" s="16" t="s">
         <v>302</v>
@@ -16981,7 +16987,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixing Nital and alltron
</commit_message>
<xml_diff>
--- a/PartnerMasterConfiguration.xlsx
+++ b/PartnerMasterConfiguration.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB49AB62-225B-4F38-9E74-DDA5A2A65055}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F68978-0B0B-4918-8891-C0E8F6588F7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -4495,11 +4495,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="7" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="7" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -4975,10 +4975,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB208"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="A173" sqref="A173"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -18759,24 +18759,24 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="86"/>
+      <c r="B8" s="87"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
       <c r="I9" t="s">
         <v>44</v>
       </c>
@@ -18785,15 +18785,15 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
       <c r="I10" t="s">
         <v>46</v>
       </c>
@@ -18802,15 +18802,15 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
       <c r="I11" t="s">
         <v>44</v>
       </c>
@@ -18832,9 +18832,9 @@
   <sheetPr codeName="Sheet3" filterMode="1"/>
   <dimension ref="A1:F1778"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1428" sqref="E1428"/>
+      <selection pane="bottomLeft" activeCell="D1788" sqref="D1788"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -26907,7 +26907,7 @@
       </c>
       <c r="E639" s="29"/>
     </row>
-    <row r="640" spans="1:5" hidden="1">
+    <row r="640" spans="1:5">
       <c r="A640" s="29" t="s">
         <v>721</v>
       </c>
@@ -26920,7 +26920,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="641" spans="1:6" hidden="1">
+    <row r="641" spans="1:6">
       <c r="A641" s="29" t="s">
         <v>721</v>
       </c>
@@ -26933,7 +26933,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="642" spans="1:6" hidden="1">
+    <row r="642" spans="1:6" ht="15.75" thickBot="1">
       <c r="A642" s="29" t="s">
         <v>721</v>
       </c>
@@ -26946,7 +26946,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="643" spans="1:6" ht="15.75" hidden="1" thickBot="1">
+    <row r="643" spans="1:6" ht="15.75" thickBot="1">
       <c r="A643" s="29" t="s">
         <v>721</v>
       </c>
@@ -26959,7 +26959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="644" spans="1:6" ht="15.75" hidden="1" thickBot="1">
+    <row r="644" spans="1:6" ht="15.75" thickBot="1">
       <c r="A644" s="29" t="s">
         <v>721</v>
       </c>
@@ -26975,7 +26975,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="645" spans="1:6" ht="15.75" hidden="1" thickBot="1">
+    <row r="645" spans="1:6" ht="15.75" thickBot="1">
       <c r="A645" s="29" t="s">
         <v>721</v>
       </c>
@@ -26988,7 +26988,7 @@
       <c r="D645" s="29"/>
       <c r="E645" s="29"/>
     </row>
-    <row r="646" spans="1:6" ht="15.75" hidden="1" thickBot="1">
+    <row r="646" spans="1:6" ht="15.75" thickBot="1">
       <c r="A646" s="29" t="s">
         <v>721</v>
       </c>
@@ -27004,7 +27004,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="647" spans="1:6" ht="15.75" hidden="1" thickBot="1">
+    <row r="647" spans="1:6" ht="15.75" thickBot="1">
       <c r="A647" s="29" t="s">
         <v>721</v>
       </c>
@@ -36209,7 +36209,7 @@
       <c r="B1316" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C1316" s="87" t="s">
+      <c r="C1316" s="86" t="s">
         <v>852</v>
       </c>
     </row>
@@ -37327,7 +37327,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1418" spans="1:6">
+    <row r="1418" spans="1:6" hidden="1">
       <c r="A1418" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37338,7 +37338,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="1419" spans="1:6">
+    <row r="1419" spans="1:6" hidden="1">
       <c r="A1419" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37349,7 +37349,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="1420" spans="1:6">
+    <row r="1420" spans="1:6" hidden="1">
       <c r="A1420" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37360,7 +37360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="1421" spans="1:6">
+    <row r="1421" spans="1:6" hidden="1">
       <c r="A1421" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37374,7 +37374,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="1422" spans="1:6">
+    <row r="1422" spans="1:6" hidden="1">
       <c r="A1422" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37385,7 +37385,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="1423" spans="1:6">
+    <row r="1423" spans="1:6" hidden="1">
       <c r="A1423" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37396,7 +37396,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="1424" spans="1:6">
+    <row r="1424" spans="1:6" hidden="1">
       <c r="A1424" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37407,7 +37407,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="1425" spans="1:5">
+    <row r="1425" spans="1:5" hidden="1">
       <c r="A1425" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37418,7 +37418,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="1426" spans="1:5">
+    <row r="1426" spans="1:5" hidden="1">
       <c r="A1426" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37429,7 +37429,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="1427" spans="1:5">
+    <row r="1427" spans="1:5" hidden="1">
       <c r="A1427" s="39" t="s">
         <v>1069</v>
       </c>
@@ -37440,7 +37440,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="1428" spans="1:5">
+    <row r="1428" spans="1:5" hidden="1">
       <c r="A1428" s="39" t="s">
         <v>1073</v>
       </c>
@@ -37451,7 +37451,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="1429" spans="1:5">
+    <row r="1429" spans="1:5" hidden="1">
       <c r="A1429" s="39" t="s">
         <v>1073</v>
       </c>
@@ -37462,7 +37462,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="1430" spans="1:5">
+    <row r="1430" spans="1:5" hidden="1">
       <c r="A1430" s="39" t="s">
         <v>1073</v>
       </c>
@@ -37473,7 +37473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="1431" spans="1:5">
+    <row r="1431" spans="1:5" hidden="1">
       <c r="A1431" s="39" t="s">
         <v>1073</v>
       </c>
@@ -37484,7 +37484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1432" spans="1:5">
+    <row r="1432" spans="1:5" hidden="1">
       <c r="A1432" s="39" t="s">
         <v>1073</v>
       </c>
@@ -37495,7 +37495,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="1433" spans="1:5">
+    <row r="1433" spans="1:5" hidden="1">
       <c r="A1433" s="39" t="s">
         <v>1073</v>
       </c>
@@ -41419,8 +41419,7 @@
   <autoFilter ref="A1:F1778" xr:uid="{32A0A4D2-FA49-40AB-B76A-75F48EB88A9F}">
     <filterColumn colId="0">
       <filters>
-        <filter val="148992_I"/>
-        <filter val="148992_P"/>
+        <filter val="3434341_C"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>